<commit_message>
updated detector parameter script
</commit_message>
<xml_diff>
--- a/data/detector_parameters.xlsx
+++ b/data/detector_parameters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Patient</t>
   </si>
@@ -28,7 +28,7 @@
     <t>num_real</t>
   </si>
   <si>
-    <t>perc_real</t>
+    <t>nspikes</t>
   </si>
   <si>
     <t>Notes</t>
@@ -242,6 +242,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -268,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -276,6 +279,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -499,7 +505,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col hidden="1" min="8" max="13" width="14.43"/>
+    <col customWidth="1" min="7" max="7" width="14.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -524,29 +530,20 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -562,6 +559,15 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -572,25 +578,70 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>50.0</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
updated example plot script
</commit_message>
<xml_diff>
--- a/data/detector_parameters.xlsx
+++ b/data/detector_parameters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Patient</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Absthresh</t>
   </si>
   <si>
-    <t>num_real</t>
+    <t>num_real (out of 50)</t>
   </si>
   <si>
     <t>nspikes</t>
@@ -43,7 +43,13 @@
     <t>HUP065</t>
   </si>
   <si>
+    <t>lots of artifact!!!</t>
+  </si>
+  <si>
     <t>HUP068</t>
+  </si>
+  <si>
+    <t>run not finished; redo check</t>
   </si>
   <si>
     <t>HUP070</t>
@@ -245,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -256,13 +262,26 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -284,11 +303,41 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -544,20 +593,59 @@
       <c r="D2" s="2">
         <v>50.0</v>
       </c>
+      <c r="E2" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2760.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2846.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4501.0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>44300.0</v>
@@ -568,15 +656,24 @@
       <c r="D5" s="2">
         <v>50.0</v>
       </c>
+      <c r="E5" s="2">
+        <v>41.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45272.0</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>44300.0</v>
@@ -590,7 +687,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <v>44300.0</v>
@@ -604,7 +701,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>44300.0</v>
@@ -618,7 +715,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3">
         <v>44300.0</v>
@@ -632,7 +729,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3">
         <v>44300.0</v>
@@ -646,295 +743,342 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>50.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>50.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>50.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44300.0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>50.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1000">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1000">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
prep for 2 new patients
</commit_message>
<xml_diff>
--- a/data/detector_parameters.xlsx
+++ b/data/detector_parameters.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
-  <si>
-    <t>Patient</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="158">
   <si>
     <t>ID</t>
   </si>
@@ -43,6 +40,9 @@
     <t>HUP060</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>bad</t>
   </si>
   <si>
@@ -52,6 +52,9 @@
     <t>HUP065</t>
   </si>
   <si>
+    <t>I am unsure about whether to call some of these spikes; they are sharply contoured fast activity, but not definitely spikes</t>
+  </si>
+  <si>
     <t>lots of artifact!!!</t>
   </si>
   <si>
@@ -67,7 +70,7 @@
     <t>HUP073</t>
   </si>
   <si>
-    <t>I am unsure about whether to call some of these spikes; they are sharply contoured fast activity, but not definitely spikes</t>
+    <t>these are funny, are they sz??</t>
   </si>
   <si>
     <t>HUP074</t>
@@ -79,6 +82,9 @@
     <t>HUP078</t>
   </si>
   <si>
+    <t>tons of artifact</t>
+  </si>
+  <si>
     <t>lots of artifact, including ekg</t>
   </si>
   <si>
@@ -88,21 +94,33 @@
     <t>HUP082</t>
   </si>
   <si>
+    <t>sz??? ekg artifact? so regular , check!!!</t>
+  </si>
+  <si>
     <t>ekg artifact, maybe sz</t>
   </si>
   <si>
     <t>HUP083</t>
   </si>
   <si>
+    <t>fast buzz of spikes, questionable whether spikes, too short to be sz (BIRD)</t>
+  </si>
+  <si>
     <t>sz???</t>
   </si>
   <si>
     <t>HUP086</t>
   </si>
   <si>
+    <t>artifact</t>
+  </si>
+  <si>
     <t>HUP087</t>
   </si>
   <si>
+    <t>sz, artifact</t>
+  </si>
+  <si>
     <t>HUP088</t>
   </si>
   <si>
@@ -133,6 +151,9 @@
     <t>HUP111A</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>empty</t>
   </si>
   <si>
@@ -151,6 +172,9 @@
     <t>HUP117</t>
   </si>
   <si>
+    <t>sz</t>
+  </si>
+  <si>
     <t>HUP123</t>
   </si>
   <si>
@@ -178,6 +202,9 @@
     <t>HUP133</t>
   </si>
   <si>
+    <t>sharply contoured activity</t>
+  </si>
+  <si>
     <t>lots of high frequency sharply contoured non spike activity</t>
   </si>
   <si>
@@ -244,6 +271,9 @@
     <t>HUP163</t>
   </si>
   <si>
+    <t>artifact and HF activity</t>
+  </si>
+  <si>
     <t>HUP164</t>
   </si>
   <si>
@@ -295,10 +325,166 @@
     <t>cool sleep example</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Patients with &gt;30/50 good</t>
+    <t>HUP081</t>
+  </si>
+  <si>
+    <t>HUP119</t>
+  </si>
+  <si>
+    <t>HUP153</t>
+  </si>
+  <si>
+    <t>HUP159</t>
+  </si>
+  <si>
+    <t>HUP167</t>
+  </si>
+  <si>
+    <t>HUP147</t>
+  </si>
+  <si>
+    <t>HUP156</t>
+  </si>
+  <si>
+    <t>HUP161</t>
+  </si>
+  <si>
+    <t>HUP178</t>
+  </si>
+  <si>
+    <t>HUP168</t>
+  </si>
+  <si>
+    <t>LVF</t>
+  </si>
+  <si>
+    <t>HUP174</t>
+  </si>
+  <si>
+    <t>HUP155</t>
+  </si>
+  <si>
+    <t>HUP186</t>
+  </si>
+  <si>
+    <t>HUP175</t>
+  </si>
+  <si>
+    <t>HUP191</t>
+  </si>
+  <si>
+    <t>HUP210</t>
+  </si>
+  <si>
+    <t>HUP183</t>
+  </si>
+  <si>
+    <t>HUP182</t>
+  </si>
+  <si>
+    <t>HUP184</t>
+  </si>
+  <si>
+    <t>HUP189</t>
+  </si>
+  <si>
+    <t>HUP196</t>
+  </si>
+  <si>
+    <t>HUP195</t>
+  </si>
+  <si>
+    <t>seizure</t>
+  </si>
+  <si>
+    <t>HUP206</t>
+  </si>
+  <si>
+    <t>HF fast</t>
+  </si>
+  <si>
+    <t>HUP197</t>
+  </si>
+  <si>
+    <t>HUP207</t>
+  </si>
+  <si>
+    <t>HUP201</t>
+  </si>
+  <si>
+    <t>HUP204</t>
+  </si>
+  <si>
+    <t>HUP202</t>
+  </si>
+  <si>
+    <t>HUP209</t>
+  </si>
+  <si>
+    <t>HUP208</t>
+  </si>
+  <si>
+    <t>HUP213</t>
+  </si>
+  <si>
+    <t>HUP211</t>
+  </si>
+  <si>
+    <t>HUP212</t>
+  </si>
+  <si>
+    <t>HUP214</t>
+  </si>
+  <si>
+    <t>HUP100</t>
+  </si>
+  <si>
+    <t>HUP101</t>
+  </si>
+  <si>
+    <t>sharp fast + artifat</t>
+  </si>
+  <si>
+    <t>HUP110</t>
+  </si>
+  <si>
+    <t>definite szs</t>
+  </si>
+  <si>
+    <t>HUP111</t>
+  </si>
+  <si>
+    <t>HUP128</t>
+  </si>
+  <si>
+    <t>HUP129</t>
+  </si>
+  <si>
+    <t>artifact, sharp fast, sz</t>
+  </si>
+  <si>
+    <t>HUP136</t>
+  </si>
+  <si>
+    <t>HUP152</t>
+  </si>
+  <si>
+    <t>HUP193</t>
+  </si>
+  <si>
+    <t>HUP198</t>
+  </si>
+  <si>
+    <t>sharp fast :(</t>
+  </si>
+  <si>
+    <t>HUP096</t>
+  </si>
+  <si>
+    <t>HUP113</t>
+  </si>
+  <si>
+    <t>HUP176</t>
   </si>
 </sst>
 </file>
@@ -318,7 +504,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -327,6 +512,9 @@
       <i/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -349,35 +537,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -624,72 +809,76 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
         <v>1.0</v>
       </c>
-      <c r="C2" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5">
+      <c r="C2" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4078.0</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3">
         <v>44300.0</v>
       </c>
       <c r="K2" s="1">
@@ -701,7 +890,7 @@
       <c r="M2" s="1">
         <v>17.0</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>2760.0</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -712,19 +901,25 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2.0</v>
       </c>
-      <c r="C3" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5">
+      <c r="C3" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4783.0</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3">
         <v>44300.0</v>
       </c>
       <c r="K3" s="1">
@@ -744,19 +939,27 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>3.0</v>
       </c>
-      <c r="C4" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5">
+      <c r="C4" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1175.0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="3">
         <v>44300.0</v>
       </c>
       <c r="K4" s="1">
@@ -772,26 +975,32 @@
         <v>4501.0</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
         <v>4.0</v>
       </c>
-      <c r="C5" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5">
+      <c r="C5" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>146527.0</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3">
         <v>44300.0</v>
       </c>
       <c r="K5" s="1">
@@ -803,52 +1012,69 @@
       <c r="M5" s="1">
         <v>45.0</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="4">
         <v>69816.0</v>
       </c>
-      <c r="O5" s="7"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2">
         <v>5.0</v>
       </c>
-      <c r="C6" s="5">
-        <v>44306.0</v>
+      <c r="C6" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>50562.0</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M6" s="1">
         <v>44.0</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="4">
         <v>29593.0</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2">
         <v>6.0</v>
       </c>
-      <c r="C7" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D7" s="1">
         <v>15.0</v>
       </c>
-      <c r="E7" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5">
+      <c r="E7" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>9967.0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="3">
         <v>44300.0</v>
       </c>
       <c r="K7" s="1">
@@ -860,30 +1086,35 @@
       <c r="M7" s="1">
         <v>20.0</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="4">
         <v>13737.0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
         <v>7.0</v>
       </c>
-      <c r="C8" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5">
+      <c r="C8" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>72449.0</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3">
         <v>44300.0</v>
       </c>
       <c r="K8" s="1">
@@ -895,31 +1126,37 @@
       <c r="M8" s="1">
         <v>37.0</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="4">
         <v>34834.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
         <v>8.0</v>
       </c>
-      <c r="C9" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D9" s="1">
         <v>21.0</v>
       </c>
-      <c r="E9" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5">
+      <c r="E9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>74165.0</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="3">
         <v>44300.0</v>
       </c>
       <c r="K9" s="1">
@@ -931,32 +1168,40 @@
       <c r="M9" s="1">
         <v>49.0</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="4">
         <v>42244.0</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2">
         <v>9.0</v>
       </c>
-      <c r="C10" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D10" s="1">
         <v>21.0</v>
       </c>
-      <c r="E10" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5">
+      <c r="E10" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>139153.0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="3">
         <v>44300.0</v>
       </c>
       <c r="K10" s="1">
@@ -968,32 +1213,38 @@
       <c r="M10" s="1">
         <v>22.0</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="4">
         <v>121330.0</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="P10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" ref="B11:B69" si="1">B10+1</f>
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" ref="B11:B103" si="1">B10+1</f>
         <v>10</v>
       </c>
-      <c r="C11" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5">
+      <c r="C11" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>47905.0</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="3">
         <v>44300.0</v>
       </c>
       <c r="K11" s="1">
@@ -1005,58 +1256,74 @@
       <c r="M11" s="1">
         <v>42.0</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="4">
         <v>24791.0</v>
       </c>
-      <c r="P11" s="6"/>
+      <c r="P11" s="4"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="3">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="C12" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45278.0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="3"/>
       <c r="M12" s="1">
         <v>16.0</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="4">
         <v>22628.0</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="P12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C13" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5">
+      <c r="C13" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>89380.0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="3">
         <v>44300.0</v>
       </c>
       <c r="K13" s="1">
@@ -1068,32 +1335,40 @@
       <c r="M13" s="1">
         <v>43.0</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="4">
         <v>44032.0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="P13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C14" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5">
+      <c r="C14" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>184199.0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="3">
         <v>44300.0</v>
       </c>
       <c r="K14" s="1">
@@ -1105,55 +1380,73 @@
       <c r="M14" s="1">
         <v>48.0</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="4">
         <v>89583.0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="P14" s="4"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C15" s="5">
-        <v>44306.0</v>
+      <c r="C15" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>9446.0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M15" s="1">
         <v>43.0</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="4">
         <v>3006.0</v>
       </c>
-      <c r="P15" s="6"/>
+      <c r="P15" s="4"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C16" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D16" s="1">
         <v>15.0</v>
       </c>
-      <c r="E16" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5">
+      <c r="E16" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>91233.0</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="3">
         <v>44300.0</v>
       </c>
       <c r="K16" s="1">
@@ -1165,29 +1458,34 @@
       <c r="M16" s="1">
         <v>43.0</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="4">
         <v>47298.0</v>
       </c>
-      <c r="P16" s="6"/>
+      <c r="P16" s="4"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="3">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C17" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5">
+      <c r="C17" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>34198.0</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="3">
         <v>44300.0</v>
       </c>
       <c r="K17" s="1">
@@ -1199,33 +1497,39 @@
       <c r="M17" s="1">
         <v>50.0</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="4">
         <v>17693.0</v>
       </c>
-      <c r="P17" s="6"/>
+      <c r="P17" s="4"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="3">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C18" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D18" s="1">
         <v>13.0</v>
       </c>
-      <c r="E18" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5">
+      <c r="E18" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>37.0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>198745.0</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="3">
         <v>44301.0</v>
       </c>
       <c r="K18" s="1">
@@ -1237,48 +1541,63 @@
       <c r="M18" s="1">
         <v>38.0</v>
       </c>
-      <c r="N18" s="6">
+      <c r="N18" s="4">
         <v>29807.0</v>
       </c>
-      <c r="P18" s="6"/>
+      <c r="P18" s="4"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C19" s="5">
-        <v>44306.0</v>
+      <c r="C19" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>87137.0</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M19" s="1">
         <v>40.0</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="4">
         <v>44654.0</v>
       </c>
-      <c r="P19" s="6"/>
+      <c r="P19" s="4"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="3">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C20" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5">
+      <c r="C20" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>90746.0</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="3">
         <v>44301.0</v>
       </c>
       <c r="K20" s="1">
@@ -1290,29 +1609,35 @@
       <c r="M20" s="1">
         <v>41.0</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="4">
         <v>43574.0</v>
       </c>
-      <c r="P20" s="6"/>
+      <c r="P20" s="4"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="3">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C21" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5">
+      <c r="C21" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="1">
+        <v>31.0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>371968.0</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="3">
         <v>44301.0</v>
       </c>
       <c r="K21" s="1">
@@ -1324,29 +1649,35 @@
       <c r="M21" s="1">
         <v>45.0</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="4">
         <v>208828.0</v>
       </c>
-      <c r="P21" s="8"/>
+      <c r="P21" s="6"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="3">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C22" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5">
+      <c r="C22" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>49715.0</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="3">
         <v>44301.0</v>
       </c>
       <c r="K22" s="1">
@@ -1358,29 +1689,35 @@
       <c r="M22" s="1">
         <v>43.0</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="4">
         <v>25937.0</v>
       </c>
-      <c r="P22" s="6"/>
+      <c r="P22" s="4"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="3">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C23" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5">
+      <c r="C23" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>94881.0</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="3">
         <v>44301.0</v>
       </c>
       <c r="K23" s="1">
@@ -1392,29 +1729,35 @@
       <c r="M23" s="1">
         <v>43.0</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="4">
         <v>47765.0</v>
       </c>
-      <c r="P23" s="6"/>
+      <c r="P23" s="4"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C24" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5">
+      <c r="C24" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>114142.0</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="3">
         <v>44301.0</v>
       </c>
       <c r="K24" s="1">
@@ -1426,51 +1769,66 @@
       <c r="M24" s="1">
         <v>40.0</v>
       </c>
-      <c r="N24" s="6">
+      <c r="N24" s="4">
         <v>69257.0</v>
       </c>
-      <c r="P24" s="6"/>
+      <c r="P24" s="4"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C25" s="5">
-        <v>44306.0</v>
+      <c r="C25" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="3">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C26" s="5">
-        <v>44306.0</v>
+      <c r="C26" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="3">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C27" s="5">
-        <v>44306.0</v>
+      <c r="C27" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M27" s="1">
         <v>0.0</v>
@@ -1478,45 +1836,60 @@
       <c r="N27" s="1">
         <v>0.0</v>
       </c>
-      <c r="P27" s="6"/>
+      <c r="P27" s="4"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="3">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C28" s="5">
-        <v>44306.0</v>
+      <c r="C28" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>92315.0</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M28" s="1">
         <v>36.0</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="4">
         <v>50898.0</v>
       </c>
-      <c r="P28" s="6"/>
+      <c r="P28" s="4"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="3">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C29" s="4">
-        <v>44306.0</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5">
+      <c r="C29" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>29731.0</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="3">
         <v>44301.0</v>
       </c>
       <c r="K29" s="1">
@@ -1528,179 +1901,254 @@
       <c r="M29" s="1">
         <v>50.0</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="4">
         <v>16039.0</v>
       </c>
-      <c r="P29" s="6"/>
+      <c r="P29" s="4"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="3">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C30" s="5">
-        <v>44306.0</v>
+      <c r="C30" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>68836.0</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M30" s="1">
         <v>44.0</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="4">
         <v>32888.0</v>
       </c>
-      <c r="P30" s="6"/>
+      <c r="P30" s="4"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="3">
+        <v>54</v>
+      </c>
+      <c r="B31" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="C31" s="5">
-        <v>44306.0</v>
+      <c r="C31" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>929822.0</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M31" s="1">
         <v>47.0</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="4">
         <v>473121.0</v>
       </c>
-      <c r="P31" s="6"/>
+      <c r="P31" s="4"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="3">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="C32" s="5">
-        <v>44306.0</v>
+      <c r="C32" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>97622.0</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M32" s="1">
         <v>8.0</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32" s="4">
         <v>51057.0</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P32" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="P32" s="4"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="3">
+        <v>57</v>
+      </c>
+      <c r="B33" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="C33" s="5">
-        <v>44306.0</v>
+      <c r="C33" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P33" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="P33" s="4"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="3">
+        <v>58</v>
+      </c>
+      <c r="B34" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C34" s="5">
-        <v>44306.0</v>
+      <c r="C34" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>286766.0</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M34" s="1">
         <v>49.0</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="4">
         <v>145929.0</v>
       </c>
-      <c r="P34" s="6"/>
+      <c r="P34" s="4"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="3">
+        <v>59</v>
+      </c>
+      <c r="B35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="C35" s="5">
-        <v>44306.0</v>
+      <c r="C35" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>139716.0</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M35" s="1">
         <v>50.0</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="4">
         <v>73965.0</v>
       </c>
-      <c r="P35" s="6"/>
+      <c r="P35" s="4"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="3">
+        <v>60</v>
+      </c>
+      <c r="B36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="C36" s="5">
-        <v>44306.0</v>
+      <c r="C36" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>191825.0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M36" s="1">
         <v>48.0</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="4">
         <v>98347.0</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P36" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="P36" s="4"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="3">
+        <v>62</v>
+      </c>
+      <c r="B37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="C37" s="5">
-        <v>44306.0</v>
+      <c r="C37" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>28580.0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M37" s="1">
         <v>35.0</v>
       </c>
-      <c r="N37" s="6">
+      <c r="N37" s="4">
         <v>14088.0</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P37" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="P37" s="4"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="3">
+        <v>65</v>
+      </c>
+      <c r="B38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="C38" s="5">
-        <v>44306.0</v>
+      <c r="C38" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D38" s="1">
         <v>21.0</v>
@@ -1708,27 +2156,39 @@
       <c r="E38" s="1">
         <v>50.0</v>
       </c>
+      <c r="F38" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>6532.0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M38" s="1">
         <v>15.0</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="4">
         <v>10262.0</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P38" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="P38" s="4"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="3">
+        <v>66</v>
+      </c>
+      <c r="B39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="C39" s="5">
-        <v>44306.0</v>
+      <c r="C39" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D39" s="1">
         <v>21.0</v>
@@ -1736,156 +2196,228 @@
       <c r="E39" s="1">
         <v>50.0</v>
       </c>
+      <c r="F39" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>23033.0</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M39" s="1">
         <v>21.0</v>
       </c>
-      <c r="N39" s="6">
+      <c r="N39" s="4">
         <v>30333.0</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P39" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="P39" s="4"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="3">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="C40" s="5">
-        <v>44306.0</v>
+      <c r="C40" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>34375.0</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M40" s="1">
         <v>36.0</v>
       </c>
-      <c r="N40" s="6">
+      <c r="N40" s="4">
         <v>20684.0</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P40" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="P40" s="4"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="3">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="C41" s="5">
-        <v>44306.0</v>
+      <c r="C41" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>150601.0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M41" s="1">
         <v>33.0</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="4">
         <v>79119.0</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P41" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="P41" s="4"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="3">
+        <v>69</v>
+      </c>
+      <c r="B42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="C42" s="5">
-        <v>44306.0</v>
+      <c r="C42" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>26145.0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M42" s="1">
         <v>46.0</v>
       </c>
-      <c r="N42" s="6">
+      <c r="N42" s="4">
         <v>10456.0</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P42" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="P42" s="4"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="3">
+        <v>71</v>
+      </c>
+      <c r="B43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="C43" s="5">
-        <v>44306.0</v>
+      <c r="C43" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>136012.0</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M43" s="1">
         <v>46.0</v>
       </c>
-      <c r="N43" s="6">
+      <c r="N43" s="4">
         <v>78393.0</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P43" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="P43" s="4"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="3">
+        <v>72</v>
+      </c>
+      <c r="B44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="C44" s="5">
-        <v>44306.0</v>
+      <c r="C44" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>224824.0</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M44" s="1">
         <v>42.0</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="4">
         <v>123171.0</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P44" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="P44" s="4"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="3">
+        <v>73</v>
+      </c>
+      <c r="B45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="C45" s="5">
-        <v>44306.0</v>
+      <c r="C45" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>37736.0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M45" s="1">
         <v>38.0</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="4">
         <v>16938.0</v>
       </c>
-      <c r="P45" s="6"/>
+      <c r="P45" s="4"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="3">
+        <v>74</v>
+      </c>
+      <c r="B46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="C46" s="5">
-        <v>44306.0</v>
+      <c r="C46" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D46" s="1">
         <v>21.0</v>
@@ -1893,131 +2425,194 @@
       <c r="E46" s="1">
         <v>50.0</v>
       </c>
+      <c r="F46" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="G46" s="4">
+        <v>9527.0</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M46" s="1">
         <v>11.0</v>
       </c>
-      <c r="N46" s="6">
+      <c r="N46" s="4">
         <v>14524.0</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P46" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="P46" s="4"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="3">
+        <v>75</v>
+      </c>
+      <c r="B47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="C47" s="5">
-        <v>44306.0</v>
+      <c r="C47" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>121224.0</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M47" s="1">
         <v>35.0</v>
       </c>
-      <c r="N47" s="6">
+      <c r="N47" s="4">
         <v>61054.0</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P47" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="P47" s="4"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="3">
+        <v>76</v>
+      </c>
+      <c r="B48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="C48" s="5">
-        <v>44306.0</v>
+      <c r="C48" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G48" s="4">
+        <v>32458.0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M48" s="1">
         <v>49.0</v>
       </c>
-      <c r="N48" s="6">
+      <c r="N48" s="4">
         <v>15524.0</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="P48" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="P48" s="4"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="3">
+        <v>78</v>
+      </c>
+      <c r="B49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="C49" s="5">
-        <v>44306.0</v>
+      <c r="C49" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>156752.0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M49" s="1">
         <v>46.0</v>
       </c>
-      <c r="N49" s="6">
+      <c r="N49" s="4">
         <v>83327.0</v>
       </c>
-      <c r="P49" s="6"/>
+      <c r="P49" s="4"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="3">
+        <v>79</v>
+      </c>
+      <c r="B50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="C50" s="5">
-        <v>44306.0</v>
+      <c r="C50" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>642448.0</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M50" s="1">
         <v>42.0</v>
       </c>
-      <c r="N50" s="6">
+      <c r="N50" s="4">
         <v>342798.0</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P50" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="P50" s="4"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" s="3">
+        <v>81</v>
+      </c>
+      <c r="B51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="C51" s="5">
-        <v>44306.0</v>
+      <c r="C51" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>240248.0</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M51" s="1">
         <v>46.0</v>
       </c>
-      <c r="N51" s="6">
+      <c r="N51" s="4">
         <v>123368.0</v>
       </c>
-      <c r="P51" s="6"/>
+      <c r="P51" s="4"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="3">
+        <v>82</v>
+      </c>
+      <c r="B52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="C52" s="5">
-        <v>44306.0</v>
+      <c r="C52" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D52" s="1">
         <v>21.0</v>
@@ -2025,27 +2620,36 @@
       <c r="E52" s="1">
         <v>50.0</v>
       </c>
+      <c r="F52" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="G52" s="4">
+        <v>22740.0</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M52" s="1">
         <v>29.0</v>
       </c>
-      <c r="N52" s="6">
+      <c r="N52" s="4">
         <v>36215.0</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P52" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P52" s="4"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="3">
+        <v>84</v>
+      </c>
+      <c r="B53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="C53" s="5">
-        <v>44306.0</v>
+      <c r="C53" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D53" s="1">
         <v>21.0</v>
@@ -2053,27 +2657,36 @@
       <c r="E53" s="1">
         <v>50.0</v>
       </c>
+      <c r="F53" s="1">
+        <v>37.0</v>
+      </c>
+      <c r="G53" s="4">
+        <v>125235.0</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M53" s="1">
         <v>21.0</v>
       </c>
-      <c r="N53" s="6">
+      <c r="N53" s="4">
         <v>144883.0</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P53" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P53" s="4"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="3">
+        <v>85</v>
+      </c>
+      <c r="B54" s="2">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="C54" s="5">
-        <v>44306.0</v>
+      <c r="C54" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D54" s="1">
         <v>21.0</v>
@@ -2081,46 +2694,76 @@
       <c r="E54" s="1">
         <v>50.0</v>
       </c>
+      <c r="F54" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="G54" s="4">
+        <v>59220.0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M54" s="1">
         <v>28.0</v>
       </c>
-      <c r="N54" s="6">
+      <c r="N54" s="4">
         <v>68393.0</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P54" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P54" s="4"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="3">
+        <v>87</v>
+      </c>
+      <c r="B55" s="2">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="C55" s="5">
-        <v>44306.0</v>
+      <c r="C55" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="G55" s="4">
+        <v>335747.0</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M55" s="1">
         <v>46.0</v>
       </c>
-      <c r="N55" s="6">
+      <c r="N55" s="4">
         <v>214741.0</v>
       </c>
-      <c r="P55" s="6"/>
+      <c r="P55" s="4"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="3">
+        <v>88</v>
+      </c>
+      <c r="B56" s="2">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="C56" s="5">
-        <v>44306.0</v>
+      <c r="C56" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="G56" s="4">
+        <v>147845.0</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M56" s="1">
         <v>34.0</v>
@@ -2129,77 +2772,104 @@
         <v>87323.0</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P56" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P56" s="4"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" s="3">
+        <v>89</v>
+      </c>
+      <c r="B57" s="2">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="C57" s="5">
-        <v>44306.0</v>
+      <c r="C57" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="G57" s="4">
+        <v>70184.0</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M57" s="1">
         <v>43.0</v>
       </c>
-      <c r="N57" s="6">
+      <c r="N57" s="4">
         <v>41956.0</v>
       </c>
-      <c r="P57" s="6"/>
+      <c r="P57" s="4"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="3">
+        <v>90</v>
+      </c>
+      <c r="B58" s="2">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="C58" s="5">
-        <v>44306.0</v>
+      <c r="C58" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="G58" s="4">
+        <v>380459.0</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M58" s="1">
         <v>33.0</v>
       </c>
-      <c r="N58" s="6">
+      <c r="N58" s="4">
         <v>236914.0</v>
       </c>
-      <c r="P58" s="6"/>
+      <c r="P58" s="4"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="3">
+        <v>91</v>
+      </c>
+      <c r="B59" s="2">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="C59" s="5">
-        <v>44306.0</v>
+      <c r="C59" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="G59" s="4">
+        <v>143117.0</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M59" s="1">
         <v>39.0</v>
       </c>
-      <c r="N59" s="6">
+      <c r="N59" s="4">
         <v>83045.0</v>
       </c>
-      <c r="P59" s="6"/>
+      <c r="P59" s="4"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="3">
+        <v>92</v>
+      </c>
+      <c r="B60" s="2">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="C60" s="5">
-        <v>44306.0</v>
+      <c r="C60" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D60" s="1">
         <v>21.0</v>
@@ -2207,46 +2877,64 @@
       <c r="E60" s="1">
         <v>50.0</v>
       </c>
+      <c r="F60" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="G60" s="4">
+        <v>3108.0</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M60" s="1">
         <v>3.0</v>
       </c>
-      <c r="N60" s="6">
+      <c r="N60" s="4">
         <v>6985.0</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P60" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P60" s="4"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="3">
+        <v>93</v>
+      </c>
+      <c r="B61" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="C61" s="5">
-        <v>44306.0</v>
+      <c r="C61" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="G61" s="4">
+        <v>120105.0</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M61" s="1">
         <v>35.0</v>
       </c>
-      <c r="N61" s="6">
+      <c r="N61" s="4">
         <v>71698.0</v>
       </c>
-      <c r="P61" s="6"/>
+      <c r="P61" s="4"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" s="3">
+        <v>94</v>
+      </c>
+      <c r="B62" s="2">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="C62" s="5">
-        <v>44306.0</v>
+      <c r="C62" s="3">
+        <v>44308.0</v>
       </c>
       <c r="D62" s="1">
         <v>21.0</v>
@@ -2254,194 +2942,886 @@
       <c r="E62" s="1">
         <v>50.0</v>
       </c>
+      <c r="F62" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="G62" s="4">
+        <v>32177.0</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="M62" s="1">
         <v>29.0</v>
       </c>
-      <c r="N62" s="6">
+      <c r="N62" s="4">
         <v>43155.0</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P62" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="P62" s="4"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="3">
+        <v>95</v>
+      </c>
+      <c r="B63" s="2">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="C63" s="5">
-        <v>44306.0</v>
+      <c r="C63" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G63" s="4">
+        <v>656232.0</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M63" s="1">
         <v>44.0</v>
       </c>
-      <c r="N63" s="6">
+      <c r="N63" s="4">
         <v>341128.0</v>
       </c>
-      <c r="P63" s="6"/>
+      <c r="P63" s="4"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B64" s="3">
+        <v>96</v>
+      </c>
+      <c r="B64" s="2">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="C64" s="5">
-        <v>44306.0</v>
+      <c r="C64" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G64" s="4">
+        <v>29361.0</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M64" s="1">
         <v>38.0</v>
       </c>
-      <c r="N64" s="6">
+      <c r="N64" s="4">
         <v>14120.0</v>
       </c>
-      <c r="P64" s="6"/>
+      <c r="P64" s="4"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" s="3">
+        <v>97</v>
+      </c>
+      <c r="B65" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="C65" s="5">
-        <v>44306.0</v>
+      <c r="C65" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="G65" s="4">
+        <v>113457.0</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M65" s="1">
         <v>40.0</v>
       </c>
-      <c r="N65" s="6">
+      <c r="N65" s="4">
         <v>73857.0</v>
       </c>
-      <c r="P65" s="6"/>
+      <c r="P65" s="4"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="3">
+        <v>98</v>
+      </c>
+      <c r="B66" s="2">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="C66" s="5">
-        <v>44306.0</v>
+      <c r="C66" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G66" s="4">
+        <v>454665.0</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M66" s="1">
         <v>38.0</v>
       </c>
-      <c r="N66" s="6">
+      <c r="N66" s="4">
         <v>267534.0</v>
       </c>
-      <c r="P66" s="6"/>
+      <c r="P66" s="4"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" s="3">
+        <v>99</v>
+      </c>
+      <c r="B67" s="2">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="C67" s="5">
-        <v>44306.0</v>
+      <c r="C67" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="G67" s="4">
+        <v>130274.0</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M67" s="1">
         <v>45.0</v>
       </c>
-      <c r="N67" s="6">
+      <c r="N67" s="4">
         <v>76907.0</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P67" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="P67" s="4"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B68" s="3">
+        <v>101</v>
+      </c>
+      <c r="B68" s="2">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="C68" s="5">
-        <v>44306.0</v>
+      <c r="C68" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="G68" s="4">
+        <v>402440.0</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M68" s="1">
         <v>45.0</v>
       </c>
-      <c r="N68" s="6">
+      <c r="N68" s="4">
         <v>184961.0</v>
       </c>
-      <c r="P68" s="6"/>
+      <c r="P68" s="4"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="3">
+        <v>102</v>
+      </c>
+      <c r="B69" s="2">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="C69" s="5">
-        <v>44306.0</v>
+      <c r="C69" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="G69" s="4">
+        <v>228145.0</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="M69" s="1">
         <v>41.0</v>
       </c>
-      <c r="N69" s="6">
+      <c r="N69" s="4">
         <v>138303.0</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P69" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="P69" s="4"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="4"/>
-      <c r="M70" s="9">
+        <v>104</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C70" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="M70" s="7">
         <f t="shared" ref="M70:N70" si="2">average(M2:M69)</f>
         <v>36.23076923</v>
       </c>
-      <c r="N70" s="9">
+      <c r="N70" s="7">
         <f t="shared" si="2"/>
         <v>79060.23077</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="M71" s="9">
+        <v>105</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="C71" s="3">
+        <v>44308.0</v>
+      </c>
+      <c r="M71" s="7">
         <f>countif(M2:M69,"&gt;30")</f>
         <v>50</v>
       </c>
     </row>
     <row r="72">
-      <c r="C72" s="4"/>
+      <c r="A72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="C72" s="3">
+        <v>44308.0</v>
+      </c>
     </row>
     <row r="73">
-      <c r="C73" s="4"/>
+      <c r="A73" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="2">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C73" s="3">
+        <v>44308.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B74" s="2">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="C74" s="3">
+        <v>44308.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B75" s="2">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C75" s="3">
+        <v>44308.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B76" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C76" s="3">
+        <v>44308.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="2">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" s="2">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="2">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="D79" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F79" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="G79" s="4">
+        <v>154752.0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I79" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="G82" s="8">
+        <v>88458.0</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" s="2">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="2">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="G87" s="8">
+        <v>444821.0</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" s="2">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="G88" s="8">
+        <v>44297.0</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" s="2">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B90" s="2">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="F91" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="G91" s="4">
+        <v>13659.0</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B92" s="2">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="F92" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="G92" s="4">
+        <v>303318.0</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B93" s="2">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="F93" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G93" s="4">
+        <v>131817.0</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B94" s="2">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B95" s="2">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="F95" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="G95" s="4">
+        <v>143248.0</v>
+      </c>
+      <c r="I95" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B96" s="2">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B97" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B98" s="2">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="F98" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="G98" s="8">
+        <v>361004.0</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B99" s="2">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B100" s="2">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B101" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102" s="2">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B103" s="2">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="1">
+        <v>103.0</v>
+      </c>
+      <c r="F104" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G104" s="4">
+        <v>198773.0</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B105" s="1">
+        <v>104.0</v>
+      </c>
+      <c r="F105" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="G105" s="4">
+        <v>26879.0</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B106" s="1">
+        <v>105.0</v>
+      </c>
+      <c r="F106" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="G106" s="4">
+        <v>93917.0</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B107" s="1">
+        <v>106.0</v>
+      </c>
+      <c r="F107" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G107" s="4">
+        <v>116076.0</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I107" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108" s="1">
+        <v>107.0</v>
+      </c>
+      <c r="F108" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="G108" s="4">
+        <v>189271.0</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I108" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109" s="1">
+        <v>108.0</v>
+      </c>
+      <c r="F109" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="G109" s="4">
+        <v>11157.0</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I109" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B110" s="1">
+        <v>109.0</v>
+      </c>
+      <c r="F110" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="G110" s="4">
+        <v>128775.0</v>
+      </c>
+      <c r="I110" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111" s="1">
+        <v>110.0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>35.0</v>
+      </c>
+      <c r="G111" s="4">
+        <v>433534.0</v>
+      </c>
+      <c r="I111" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B112" s="1">
+        <v>111.0</v>
+      </c>
+      <c r="F112" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G112" s="4">
+        <v>49224.0</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I112" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B113" s="1">
+        <v>112.0</v>
+      </c>
+      <c r="D113" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="E113" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F113" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G113" s="4">
+        <v>80467.0</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I113" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B114" s="1">
+        <v>113.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B115" s="1">
+        <v>114.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B116" s="1">
+        <v>115.0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1 M1:M1000">
+  <conditionalFormatting sqref="F1:F1000 M1:M1000">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 M1:M20 P21 M22:M1000">
+  <conditionalFormatting sqref="F1:F1000 M1:M20 P21 M22:M1000">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
switched bipolar to car
</commit_message>
<xml_diff>
--- a/data/detector_parameters.xlsx
+++ b/data/detector_parameters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="159">
   <si>
     <t>Patient</t>
   </si>
@@ -541,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -552,6 +552,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -812,7 +815,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="15" max="15" width="14.86"/>
+    <col customWidth="1" min="22" max="22" width="14.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -822,25 +825,25 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -862,6 +865,27 @@
         <v>7</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -873,36 +897,45 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="4">
-        <v>44308.0</v>
+        <v>44316.0</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="2">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="2">
         <v>24.0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="N2" s="6">
         <v>4078.0</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="O2" s="5"/>
+      <c r="P2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="R2" s="2">
         <v>17.0</v>
       </c>
-      <c r="L2" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="S2" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T2" s="2">
         <v>17.0</v>
       </c>
-      <c r="N2" s="5">
+      <c r="U2" s="6">
         <v>2760.0</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -913,34 +946,41 @@
       <c r="B3" s="3">
         <v>2.0</v>
       </c>
-      <c r="C3" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="2">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="2">
         <v>40.0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="N3" s="6">
         <v>4783.0</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="O3" s="5"/>
+      <c r="P3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K3" s="2">
+      <c r="R3" s="2">
         <v>17.0</v>
       </c>
-      <c r="L3" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="S3" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T3" s="2">
         <v>35.0</v>
       </c>
-      <c r="N3" s="2">
+      <c r="U3" s="2">
         <v>2846.0</v>
       </c>
     </row>
@@ -951,39 +991,46 @@
       <c r="B4" s="3">
         <v>3.0</v>
       </c>
-      <c r="C4" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="2">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="2">
         <v>29.0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="N4" s="6">
         <v>1175.0</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="P4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K4" s="2">
+      <c r="R4" s="2">
         <v>17.0</v>
       </c>
-      <c r="L4" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="S4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T4" s="2">
         <v>7.0</v>
       </c>
-      <c r="N4" s="2">
+      <c r="U4" s="2">
         <v>4501.0</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -994,37 +1041,44 @@
       <c r="B5" s="3">
         <v>4.0</v>
       </c>
-      <c r="C5" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="2">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="2">
         <v>48.0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="N5" s="6">
         <v>146527.0</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="O5" s="5"/>
+      <c r="P5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K5" s="2">
+      <c r="R5" s="2">
         <v>17.0</v>
       </c>
-      <c r="L5" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="S5" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T5" s="2">
         <v>45.0</v>
       </c>
-      <c r="N5" s="5">
+      <c r="U5" s="6">
         <v>69816.0</v>
       </c>
-      <c r="O5" s="6"/>
+      <c r="V5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -1033,25 +1087,30 @@
       <c r="B6" s="3">
         <v>5.0</v>
       </c>
-      <c r="C6" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M6" s="2">
         <v>42.0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="N6" s="6">
         <v>50562.0</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="P6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="2">
         <v>44.0</v>
       </c>
-      <c r="N6" s="5">
+      <c r="U6" s="6">
         <v>29593.0</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1062,43 +1121,54 @@
       <c r="B7" s="3">
         <v>6.0</v>
       </c>
-      <c r="C7" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="5"/>
+      <c r="D7" s="1">
         <v>15.0</v>
       </c>
-      <c r="E7" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M7" s="2">
         <v>48.0</v>
       </c>
-      <c r="G7" s="5">
+      <c r="N7" s="6">
         <v>9967.0</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="P7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K7" s="2">
+      <c r="R7" s="2">
         <v>13.0</v>
       </c>
-      <c r="L7" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="S7" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T7" s="2">
         <v>20.0</v>
       </c>
-      <c r="N7" s="5">
+      <c r="U7" s="6">
         <v>13737.0</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1109,33 +1179,40 @@
       <c r="B8" s="3">
         <v>7.0</v>
       </c>
-      <c r="C8" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="2">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="2">
         <v>47.0</v>
       </c>
-      <c r="G8" s="5">
+      <c r="N8" s="6">
         <v>72449.0</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="P8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K8" s="2">
+      <c r="R8" s="2">
         <v>17.0</v>
       </c>
-      <c r="L8" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M8" s="2">
+      <c r="S8" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T8" s="2">
         <v>37.0</v>
       </c>
-      <c r="N8" s="5">
+      <c r="U8" s="6">
         <v>34834.0</v>
       </c>
     </row>
@@ -1146,27 +1223,19 @@
       <c r="B9" s="3">
         <v>8.0</v>
       </c>
-      <c r="C9" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="5"/>
+      <c r="D9" s="1">
         <v>21.0</v>
       </c>
-      <c r="E9" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>49.0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>74165.0</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="4">
-        <v>44300.0</v>
+      <c r="E9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5">
+        <v>44308.0</v>
       </c>
       <c r="K9" s="2">
         <v>21.0</v>
@@ -1177,10 +1246,29 @@
       <c r="M9" s="2">
         <v>49.0</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="6">
+        <v>74165.0</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>44300.0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>49.0</v>
+      </c>
+      <c r="U9" s="6">
         <v>42244.0</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="W9" s="6"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1189,46 +1277,57 @@
       <c r="B10" s="3">
         <v>9.0</v>
       </c>
-      <c r="C10" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="5"/>
+      <c r="D10" s="1">
         <v>21.0</v>
       </c>
-      <c r="E10" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M10" s="2">
         <v>18.0</v>
       </c>
-      <c r="G10" s="5">
+      <c r="N10" s="6">
         <v>139153.0</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="P10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K10" s="2">
+      <c r="R10" s="2">
         <v>17.0</v>
       </c>
-      <c r="L10" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M10" s="2">
+      <c r="S10" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T10" s="2">
         <v>22.0</v>
       </c>
-      <c r="N10" s="5">
+      <c r="U10" s="6">
         <v>121330.0</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="W10" s="6"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -1238,37 +1337,44 @@
         <f t="shared" ref="B11:B103" si="1">B10+1</f>
         <v>10</v>
       </c>
-      <c r="C11" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="N11" s="6">
         <v>47905.0</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="O11" s="5"/>
+      <c r="P11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K11" s="2">
+      <c r="R11" s="2">
         <v>17.0</v>
       </c>
-      <c r="L11" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M11" s="2">
+      <c r="S11" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T11" s="2">
         <v>42.0</v>
       </c>
-      <c r="N11" s="5">
+      <c r="U11" s="6">
         <v>24791.0</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="W11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -1278,34 +1384,41 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="2">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="2">
         <v>36.0</v>
       </c>
-      <c r="G12" s="5">
+      <c r="N12" s="6">
         <v>45278.0</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="M12" s="2">
+      <c r="P12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="T12" s="2">
         <v>16.0</v>
       </c>
-      <c r="N12" s="5">
+      <c r="U12" s="6">
         <v>22628.0</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="W12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
@@ -1315,42 +1428,49 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C13" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="2">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="2">
         <v>45.0</v>
       </c>
-      <c r="G13" s="5">
+      <c r="N13" s="6">
         <v>89380.0</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="P13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K13" s="2">
+      <c r="R13" s="2">
         <v>17.0</v>
       </c>
-      <c r="L13" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M13" s="2">
+      <c r="S13" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T13" s="2">
         <v>43.0</v>
       </c>
-      <c r="N13" s="5">
+      <c r="U13" s="6">
         <v>44032.0</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="V13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="W13" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1360,42 +1480,49 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C14" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="2">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="2">
         <v>46.0</v>
       </c>
-      <c r="G14" s="5">
+      <c r="N14" s="6">
         <v>184199.0</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="P14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K14" s="2">
+      <c r="R14" s="2">
         <v>17.0</v>
       </c>
-      <c r="L14" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M14" s="2">
+      <c r="S14" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T14" s="2">
         <v>48.0</v>
       </c>
-      <c r="N14" s="5">
+      <c r="U14" s="6">
         <v>89583.0</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P14" s="5"/>
+      <c r="W14" s="6"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -1405,28 +1532,33 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C15" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M15" s="2">
         <v>39.0</v>
       </c>
-      <c r="G15" s="5">
+      <c r="N15" s="6">
         <v>9446.0</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="2">
+      <c r="P15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T15" s="2">
         <v>43.0</v>
       </c>
-      <c r="N15" s="5">
+      <c r="U15" s="6">
         <v>3006.0</v>
       </c>
-      <c r="P15" s="5"/>
+      <c r="W15" s="6"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -1436,27 +1568,19 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C16" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="5"/>
+      <c r="D16" s="1">
         <v>15.0</v>
       </c>
-      <c r="E16" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>42.0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>91233.0</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="4">
-        <v>44300.0</v>
+      <c r="E16" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5">
+        <v>44308.0</v>
       </c>
       <c r="K16" s="2">
         <v>15.0</v>
@@ -1465,12 +1589,31 @@
         <v>50.0</v>
       </c>
       <c r="M16" s="2">
+        <v>42.0</v>
+      </c>
+      <c r="N16" s="6">
+        <v>91233.0</v>
+      </c>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>44300.0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="S16" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T16" s="2">
         <v>43.0</v>
       </c>
-      <c r="N16" s="5">
+      <c r="U16" s="6">
         <v>47298.0</v>
       </c>
-      <c r="P16" s="5"/>
+      <c r="W16" s="6"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -1480,36 +1623,43 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C17" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="2">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="2">
         <v>49.0</v>
       </c>
-      <c r="G17" s="5">
+      <c r="N17" s="6">
         <v>34198.0</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="P17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="5">
         <v>44300.0</v>
       </c>
-      <c r="K17" s="2">
+      <c r="R17" s="2">
         <v>17.0</v>
       </c>
-      <c r="L17" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="N17" s="5">
+      <c r="S17" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="U17" s="6">
         <v>17693.0</v>
       </c>
-      <c r="P17" s="5"/>
+      <c r="W17" s="6"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -1519,27 +1669,19 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C18" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="5"/>
+      <c r="D18" s="1">
         <v>13.0</v>
       </c>
-      <c r="E18" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>37.0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>198745.0</v>
-      </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="4">
-        <v>44301.0</v>
+      <c r="E18" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5">
+        <v>44308.0</v>
       </c>
       <c r="K18" s="2">
         <v>13.0</v>
@@ -1548,12 +1690,31 @@
         <v>50.0</v>
       </c>
       <c r="M18" s="2">
+        <v>37.0</v>
+      </c>
+      <c r="N18" s="6">
+        <v>198745.0</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>44301.0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="S18" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T18" s="2">
         <v>38.0</v>
       </c>
-      <c r="N18" s="5">
+      <c r="U18" s="6">
         <v>29807.0</v>
       </c>
-      <c r="P18" s="5"/>
+      <c r="W18" s="6"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
@@ -1563,25 +1724,30 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C19" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="C19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M19" s="2">
         <v>33.0</v>
       </c>
-      <c r="G19" s="5">
+      <c r="N19" s="6">
         <v>87137.0</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" s="2">
+      <c r="P19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="2">
         <v>40.0</v>
       </c>
-      <c r="N19" s="5">
+      <c r="U19" s="6">
         <v>44654.0</v>
       </c>
-      <c r="P19" s="5"/>
+      <c r="W19" s="6"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -1591,37 +1757,44 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C20" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="2">
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="2">
         <v>33.0</v>
       </c>
-      <c r="G20" s="5">
+      <c r="N20" s="6">
         <v>90746.0</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="4">
+      <c r="O20" s="5"/>
+      <c r="P20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="R20" s="2">
         <v>17.0</v>
       </c>
-      <c r="L20" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M20" s="2">
+      <c r="S20" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T20" s="2">
         <v>41.0</v>
       </c>
-      <c r="N20" s="5">
+      <c r="U20" s="6">
         <v>43574.0</v>
       </c>
-      <c r="P20" s="5"/>
+      <c r="W20" s="6"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
@@ -1631,37 +1804,44 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C21" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="2">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="2">
         <v>31.0</v>
       </c>
-      <c r="G21" s="5">
+      <c r="N21" s="6">
         <v>371968.0</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="4">
+      <c r="O21" s="5"/>
+      <c r="P21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K21" s="2">
+      <c r="R21" s="2">
         <v>17.0</v>
       </c>
-      <c r="L21" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M21" s="2">
+      <c r="S21" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T21" s="2">
         <v>45.0</v>
       </c>
-      <c r="N21" s="5">
+      <c r="U21" s="6">
         <v>208828.0</v>
       </c>
-      <c r="P21" s="7"/>
+      <c r="W21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -1671,37 +1851,44 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C22" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="2">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="2">
         <v>41.0</v>
       </c>
-      <c r="G22" s="5">
+      <c r="N22" s="6">
         <v>49715.0</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="4">
+      <c r="O22" s="5"/>
+      <c r="P22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K22" s="2">
+      <c r="R22" s="2">
         <v>17.0</v>
       </c>
-      <c r="L22" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M22" s="2">
+      <c r="S22" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T22" s="2">
         <v>43.0</v>
       </c>
-      <c r="N22" s="5">
+      <c r="U22" s="6">
         <v>25937.0</v>
       </c>
-      <c r="P22" s="5"/>
+      <c r="W22" s="6"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -1711,37 +1898,44 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C23" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="2">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="2">
         <v>36.0</v>
       </c>
-      <c r="G23" s="5">
+      <c r="N23" s="6">
         <v>94881.0</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="4">
+      <c r="O23" s="5"/>
+      <c r="P23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="R23" s="2">
         <v>17.0</v>
       </c>
-      <c r="L23" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M23" s="2">
+      <c r="S23" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T23" s="2">
         <v>43.0</v>
       </c>
-      <c r="N23" s="5">
+      <c r="U23" s="6">
         <v>47765.0</v>
       </c>
-      <c r="P23" s="5"/>
+      <c r="W23" s="6"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
@@ -1751,37 +1945,44 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C24" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="2">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="2">
         <v>35.0</v>
       </c>
-      <c r="G24" s="5">
+      <c r="N24" s="6">
         <v>114142.0</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="O24" s="5"/>
+      <c r="P24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K24" s="2">
+      <c r="R24" s="2">
         <v>17.0</v>
       </c>
-      <c r="L24" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M24" s="2">
+      <c r="S24" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T24" s="2">
         <v>40.0</v>
       </c>
-      <c r="N24" s="5">
+      <c r="U24" s="6">
         <v>69257.0</v>
       </c>
-      <c r="P24" s="5"/>
+      <c r="W24" s="6"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -1791,13 +1992,18 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C25" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="I25" s="5" t="s">
+      <c r="C25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="P25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="V25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1809,13 +2015,18 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C26" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="I26" s="5" t="s">
+      <c r="C26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="P26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="V26" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1827,17 +2038,13 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C27" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>10</v>
+      <c r="C27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5">
+        <v>44308.0</v>
       </c>
       <c r="M27" s="2">
         <v>0.0</v>
@@ -1845,7 +2052,16 @@
       <c r="N27" s="2">
         <v>0.0</v>
       </c>
-      <c r="P27" s="5"/>
+      <c r="P27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T27" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W27" s="6"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
@@ -1855,25 +2071,30 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C28" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>36.0</v>
-      </c>
-      <c r="G28" s="5">
-        <v>92315.0</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>10</v>
+      <c r="C28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5">
+        <v>44308.0</v>
       </c>
       <c r="M28" s="2">
         <v>36.0</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="6">
+        <v>92315.0</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T28" s="2">
+        <v>36.0</v>
+      </c>
+      <c r="U28" s="6">
         <v>50898.0</v>
       </c>
-      <c r="P28" s="5"/>
+      <c r="W28" s="6"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
@@ -1883,37 +2104,44 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C29" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="2">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="2">
         <v>46.0</v>
       </c>
-      <c r="G29" s="5">
+      <c r="N29" s="6">
         <v>29731.0</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="4">
+      <c r="O29" s="5"/>
+      <c r="P29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="5">
         <v>44301.0</v>
       </c>
-      <c r="K29" s="2">
+      <c r="R29" s="2">
         <v>17.0</v>
       </c>
-      <c r="L29" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="M29" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="N29" s="5">
+      <c r="S29" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="T29" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="U29" s="6">
         <v>16039.0</v>
       </c>
-      <c r="P29" s="5"/>
+      <c r="W29" s="6"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
@@ -1923,28 +2151,33 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C30" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="C30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M30" s="2">
         <v>45.0</v>
       </c>
-      <c r="G30" s="5">
+      <c r="N30" s="6">
         <v>68836.0</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" s="2">
+      <c r="P30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T30" s="2">
         <v>44.0</v>
       </c>
-      <c r="N30" s="5">
+      <c r="U30" s="6">
         <v>32888.0</v>
       </c>
-      <c r="P30" s="5"/>
+      <c r="W30" s="6"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
@@ -1954,25 +2187,30 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="C31" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="C31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M31" s="2">
         <v>48.0</v>
       </c>
-      <c r="G31" s="5">
+      <c r="N31" s="6">
         <v>929822.0</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M31" s="2">
+      <c r="P31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T31" s="2">
         <v>47.0</v>
       </c>
-      <c r="N31" s="5">
+      <c r="U31" s="6">
         <v>473121.0</v>
       </c>
-      <c r="P31" s="5"/>
+      <c r="W31" s="6"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
@@ -1982,28 +2220,33 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="C32" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="C32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M32" s="2">
         <v>4.0</v>
       </c>
-      <c r="G32" s="5">
+      <c r="N32" s="6">
         <v>97622.0</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="2">
+      <c r="P32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T32" s="2">
         <v>8.0</v>
       </c>
-      <c r="N32" s="5">
+      <c r="U32" s="6">
         <v>51057.0</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="V32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="P32" s="5"/>
+      <c r="W32" s="6"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
@@ -2013,16 +2256,21 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="C33" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="I33" s="5" t="s">
+      <c r="C33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="P33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="V33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P33" s="5"/>
+      <c r="W33" s="6"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
@@ -2032,25 +2280,30 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C34" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F34" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="G34" s="5">
+      <c r="C34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="N34" s="6">
         <v>286766.0</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="2">
+      <c r="P34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T34" s="2">
         <v>49.0</v>
       </c>
-      <c r="N34" s="5">
+      <c r="U34" s="6">
         <v>145929.0</v>
       </c>
-      <c r="P34" s="5"/>
+      <c r="W34" s="6"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
@@ -2060,25 +2313,30 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="C35" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F35" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="G35" s="5">
+      <c r="C35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="N35" s="6">
         <v>139716.0</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M35" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="N35" s="5">
+      <c r="P35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="U35" s="6">
         <v>73965.0</v>
       </c>
-      <c r="P35" s="5"/>
+      <c r="W35" s="6"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
@@ -2088,31 +2346,36 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="C36" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F36" s="2">
+      <c r="C36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M36" s="2">
         <v>47.0</v>
       </c>
-      <c r="G36" s="5">
+      <c r="N36" s="6">
         <v>191825.0</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" s="2">
+      <c r="P36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="2">
         <v>48.0</v>
       </c>
-      <c r="N36" s="5">
+      <c r="U36" s="6">
         <v>98347.0</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="V36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P36" s="5"/>
+      <c r="W36" s="6"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
@@ -2122,31 +2385,36 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="C37" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F37" s="2">
+      <c r="C37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M37" s="2">
         <v>30.0</v>
       </c>
-      <c r="G37" s="5">
+      <c r="N37" s="6">
         <v>28580.0</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M37" s="2">
+      <c r="P37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="2">
         <v>35.0</v>
       </c>
-      <c r="N37" s="5">
+      <c r="U37" s="6">
         <v>14088.0</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="V37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P37" s="5"/>
+      <c r="W37" s="6"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
@@ -2156,37 +2424,48 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="C38" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="5"/>
+      <c r="D38" s="1">
         <v>21.0</v>
       </c>
-      <c r="E38" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F38" s="2">
+      <c r="E38" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L38" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M38" s="2">
         <v>27.0</v>
       </c>
-      <c r="G38" s="5">
+      <c r="N38" s="6">
         <v>6532.0</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M38" s="2">
+      <c r="P38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T38" s="2">
         <v>15.0</v>
       </c>
-      <c r="N38" s="5">
+      <c r="U38" s="6">
         <v>10262.0</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="V38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P38" s="5"/>
+      <c r="W38" s="6"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
@@ -2196,34 +2475,45 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="C39" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="C39" s="5"/>
+      <c r="D39" s="1">
         <v>21.0</v>
       </c>
-      <c r="E39" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F39" s="2">
+      <c r="E39" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L39" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M39" s="2">
         <v>39.0</v>
       </c>
-      <c r="G39" s="5">
+      <c r="N39" s="6">
         <v>23033.0</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M39" s="2">
+      <c r="P39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T39" s="2">
         <v>21.0</v>
       </c>
-      <c r="N39" s="5">
+      <c r="U39" s="6">
         <v>30333.0</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="V39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P39" s="5"/>
+      <c r="W39" s="6"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
@@ -2233,28 +2523,33 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="C40" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F40" s="2">
+      <c r="C40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M40" s="2">
         <v>42.0</v>
       </c>
-      <c r="G40" s="5">
+      <c r="N40" s="6">
         <v>34375.0</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M40" s="2">
+      <c r="P40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T40" s="2">
         <v>36.0</v>
       </c>
-      <c r="N40" s="5">
+      <c r="U40" s="6">
         <v>20684.0</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="P40" s="5"/>
+      <c r="W40" s="6"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
@@ -2264,31 +2559,36 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="C41" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F41" s="2">
+      <c r="C41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M41" s="2">
         <v>43.0</v>
       </c>
-      <c r="G41" s="5">
+      <c r="N41" s="6">
         <v>150601.0</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M41" s="2">
+      <c r="P41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T41" s="2">
         <v>33.0</v>
       </c>
-      <c r="N41" s="5">
+      <c r="U41" s="6">
         <v>79119.0</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="P41" s="5"/>
+      <c r="W41" s="6"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
@@ -2298,31 +2598,36 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="C42" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F42" s="2">
+      <c r="C42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M42" s="2">
         <v>43.0</v>
       </c>
-      <c r="G42" s="5">
+      <c r="N42" s="6">
         <v>26145.0</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M42" s="2">
+      <c r="P42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T42" s="2">
         <v>46.0</v>
       </c>
-      <c r="N42" s="5">
+      <c r="U42" s="6">
         <v>10456.0</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="V42" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P42" s="5"/>
+      <c r="W42" s="6"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
@@ -2332,28 +2637,33 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="C43" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F43" s="2">
-        <v>46.0</v>
-      </c>
-      <c r="G43" s="5">
-        <v>136012.0</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>10</v>
+      <c r="C43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5">
+        <v>44308.0</v>
       </c>
       <c r="M43" s="2">
         <v>46.0</v>
       </c>
-      <c r="N43" s="5">
+      <c r="N43" s="6">
+        <v>136012.0</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T43" s="2">
+        <v>46.0</v>
+      </c>
+      <c r="U43" s="6">
         <v>78393.0</v>
       </c>
-      <c r="O43" s="2" t="s">
+      <c r="V43" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P43" s="5"/>
+      <c r="W43" s="6"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
@@ -2363,28 +2673,33 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="C44" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="C44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M44" s="2">
         <v>48.0</v>
       </c>
-      <c r="G44" s="5">
+      <c r="N44" s="6">
         <v>224824.0</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M44" s="2">
+      <c r="P44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T44" s="2">
         <v>42.0</v>
       </c>
-      <c r="N44" s="5">
+      <c r="U44" s="6">
         <v>123171.0</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="V44" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P44" s="5"/>
+      <c r="W44" s="6"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
@@ -2394,28 +2709,33 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="C45" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="C45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M45" s="2">
         <v>34.0</v>
       </c>
-      <c r="G45" s="5">
+      <c r="N45" s="6">
         <v>37736.0</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M45" s="2">
+      <c r="P45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T45" s="2">
         <v>38.0</v>
       </c>
-      <c r="N45" s="5">
+      <c r="U45" s="6">
         <v>16938.0</v>
       </c>
-      <c r="P45" s="5"/>
+      <c r="W45" s="6"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
@@ -2425,34 +2745,45 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="C46" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="C46" s="5"/>
+      <c r="D46" s="1">
         <v>21.0</v>
       </c>
-      <c r="E46" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F46" s="2">
+      <c r="E46" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L46" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M46" s="2">
         <v>35.0</v>
       </c>
-      <c r="G46" s="5">
+      <c r="N46" s="6">
         <v>9527.0</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M46" s="2">
+      <c r="P46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T46" s="2">
         <v>11.0</v>
       </c>
-      <c r="N46" s="5">
+      <c r="U46" s="6">
         <v>14524.0</v>
       </c>
-      <c r="O46" s="2" t="s">
+      <c r="V46" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P46" s="5"/>
+      <c r="W46" s="6"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
@@ -2462,31 +2793,36 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="C47" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F47" s="2">
+      <c r="C47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M47" s="2">
         <v>32.0</v>
       </c>
-      <c r="G47" s="5">
+      <c r="N47" s="6">
         <v>121224.0</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M47" s="2">
+      <c r="P47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T47" s="2">
         <v>35.0</v>
       </c>
-      <c r="N47" s="5">
+      <c r="U47" s="6">
         <v>61054.0</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="V47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P47" s="5"/>
+      <c r="W47" s="6"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
@@ -2496,31 +2832,36 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="C48" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F48" s="2">
+      <c r="C48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M48" s="2">
         <v>45.0</v>
       </c>
-      <c r="G48" s="5">
+      <c r="N48" s="6">
         <v>32458.0</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M48" s="2">
+      <c r="P48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T48" s="2">
         <v>49.0</v>
       </c>
-      <c r="N48" s="5">
+      <c r="U48" s="6">
         <v>15524.0</v>
       </c>
-      <c r="O48" s="2" t="s">
+      <c r="V48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P48" s="5"/>
+      <c r="W48" s="6"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
@@ -2530,28 +2871,33 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="C49" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F49" s="2">
+      <c r="C49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M49" s="2">
         <v>48.0</v>
       </c>
-      <c r="G49" s="5">
+      <c r="N49" s="6">
         <v>156752.0</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I49" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M49" s="2">
+      <c r="P49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T49" s="2">
         <v>46.0</v>
       </c>
-      <c r="N49" s="5">
+      <c r="U49" s="6">
         <v>83327.0</v>
       </c>
-      <c r="P49" s="5"/>
+      <c r="W49" s="6"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
@@ -2561,28 +2907,33 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="C50" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="C50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M50" s="2">
         <v>39.0</v>
       </c>
-      <c r="G50" s="5">
+      <c r="N50" s="6">
         <v>642448.0</v>
       </c>
-      <c r="I50" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="2">
+      <c r="P50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T50" s="2">
         <v>42.0</v>
       </c>
-      <c r="N50" s="5">
+      <c r="U50" s="6">
         <v>342798.0</v>
       </c>
-      <c r="O50" s="2" t="s">
+      <c r="V50" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P50" s="5"/>
+      <c r="W50" s="6"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
@@ -2592,25 +2943,30 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="C51" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="C51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M51" s="2">
         <v>43.0</v>
       </c>
-      <c r="G51" s="5">
+      <c r="N51" s="6">
         <v>240248.0</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M51" s="2">
+      <c r="P51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T51" s="2">
         <v>46.0</v>
       </c>
-      <c r="N51" s="5">
+      <c r="U51" s="6">
         <v>123368.0</v>
       </c>
-      <c r="P51" s="5"/>
+      <c r="W51" s="6"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
@@ -2620,34 +2976,45 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="C52" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D52" s="2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="1">
         <v>21.0</v>
       </c>
-      <c r="E52" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F52" s="2">
+      <c r="E52" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K52" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L52" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M52" s="2">
         <v>33.0</v>
       </c>
-      <c r="G52" s="5">
+      <c r="N52" s="6">
         <v>22740.0</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M52" s="2">
+      <c r="P52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T52" s="2">
         <v>29.0</v>
       </c>
-      <c r="N52" s="5">
+      <c r="U52" s="6">
         <v>36215.0</v>
       </c>
-      <c r="O52" s="2" t="s">
+      <c r="V52" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P52" s="5"/>
+      <c r="W52" s="6"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
@@ -2657,34 +3024,45 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="C53" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D53" s="2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="1">
         <v>21.0</v>
       </c>
-      <c r="E53" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F53" s="2">
+      <c r="E53" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K53" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L53" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M53" s="2">
         <v>37.0</v>
       </c>
-      <c r="G53" s="5">
+      <c r="N53" s="6">
         <v>125235.0</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M53" s="2">
+      <c r="P53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T53" s="2">
         <v>21.0</v>
       </c>
-      <c r="N53" s="5">
+      <c r="U53" s="6">
         <v>144883.0</v>
       </c>
-      <c r="O53" s="2" t="s">
+      <c r="V53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P53" s="5"/>
+      <c r="W53" s="6"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
@@ -2694,37 +3072,48 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="C54" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D54" s="2">
+      <c r="C54" s="5"/>
+      <c r="D54" s="1">
         <v>21.0</v>
       </c>
-      <c r="E54" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F54" s="2">
+      <c r="E54" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K54" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L54" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M54" s="2">
         <v>29.0</v>
       </c>
-      <c r="G54" s="5">
+      <c r="N54" s="6">
         <v>59220.0</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="O54" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I54" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M54" s="2">
+      <c r="P54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T54" s="2">
         <v>28.0</v>
       </c>
-      <c r="N54" s="5">
+      <c r="U54" s="6">
         <v>68393.0</v>
       </c>
-      <c r="O54" s="2" t="s">
+      <c r="V54" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P54" s="5"/>
+      <c r="W54" s="6"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
@@ -2734,25 +3123,30 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="C55" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F55" s="2">
+      <c r="C55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M55" s="2">
         <v>49.0</v>
       </c>
-      <c r="G55" s="5">
+      <c r="N55" s="6">
         <v>335747.0</v>
       </c>
-      <c r="I55" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M55" s="2">
+      <c r="P55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T55" s="2">
         <v>46.0</v>
       </c>
-      <c r="N55" s="5">
+      <c r="U55" s="6">
         <v>214741.0</v>
       </c>
-      <c r="P55" s="5"/>
+      <c r="W55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
@@ -2762,28 +3156,33 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="C56" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F56" s="2">
+      <c r="C56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M56" s="2">
         <v>25.0</v>
       </c>
-      <c r="G56" s="5">
+      <c r="N56" s="6">
         <v>147845.0</v>
       </c>
-      <c r="I56" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M56" s="2">
+      <c r="P56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T56" s="2">
         <v>34.0</v>
       </c>
-      <c r="N56" s="2">
+      <c r="U56" s="2">
         <v>87323.0</v>
       </c>
-      <c r="O56" s="2" t="s">
+      <c r="V56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P56" s="5"/>
+      <c r="W56" s="6"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
@@ -2793,25 +3192,30 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="C57" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F57" s="2">
+      <c r="C57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M57" s="2">
         <v>39.0</v>
       </c>
-      <c r="G57" s="5">
+      <c r="N57" s="6">
         <v>70184.0</v>
       </c>
-      <c r="I57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M57" s="2">
+      <c r="P57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T57" s="2">
         <v>43.0</v>
       </c>
-      <c r="N57" s="5">
+      <c r="U57" s="6">
         <v>41956.0</v>
       </c>
-      <c r="P57" s="5"/>
+      <c r="W57" s="6"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
@@ -2821,25 +3225,30 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="C58" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F58" s="2">
+      <c r="C58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M58" s="2">
         <v>40.0</v>
       </c>
-      <c r="G58" s="5">
+      <c r="N58" s="6">
         <v>380459.0</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M58" s="2">
+      <c r="P58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T58" s="2">
         <v>33.0</v>
       </c>
-      <c r="N58" s="5">
+      <c r="U58" s="6">
         <v>236914.0</v>
       </c>
-      <c r="P58" s="5"/>
+      <c r="W58" s="6"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
@@ -2849,25 +3258,30 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="C59" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F59" s="2">
+      <c r="C59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M59" s="2">
         <v>46.0</v>
       </c>
-      <c r="G59" s="5">
+      <c r="N59" s="6">
         <v>143117.0</v>
       </c>
-      <c r="I59" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M59" s="2">
+      <c r="P59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T59" s="2">
         <v>39.0</v>
       </c>
-      <c r="N59" s="5">
+      <c r="U59" s="6">
         <v>83045.0</v>
       </c>
-      <c r="P59" s="5"/>
+      <c r="W59" s="6"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
@@ -2877,34 +3291,45 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="C60" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D60" s="2">
+      <c r="C60" s="5"/>
+      <c r="D60" s="1">
         <v>21.0</v>
       </c>
-      <c r="E60" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F60" s="2">
+      <c r="E60" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K60" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L60" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M60" s="2">
         <v>14.0</v>
       </c>
-      <c r="G60" s="5">
+      <c r="N60" s="6">
         <v>3108.0</v>
       </c>
-      <c r="I60" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M60" s="2">
+      <c r="P60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T60" s="2">
         <v>3.0</v>
       </c>
-      <c r="N60" s="5">
+      <c r="U60" s="6">
         <v>6985.0</v>
       </c>
-      <c r="O60" s="2" t="s">
+      <c r="V60" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P60" s="5"/>
+      <c r="W60" s="6"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
@@ -2914,25 +3339,30 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="C61" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F61" s="2">
+      <c r="C61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M61" s="2">
         <v>41.0</v>
       </c>
-      <c r="G61" s="5">
+      <c r="N61" s="6">
         <v>120105.0</v>
       </c>
-      <c r="I61" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M61" s="2">
+      <c r="P61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T61" s="2">
         <v>35.0</v>
       </c>
-      <c r="N61" s="5">
+      <c r="U61" s="6">
         <v>71698.0</v>
       </c>
-      <c r="P61" s="5"/>
+      <c r="W61" s="6"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
@@ -2942,34 +3372,45 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="C62" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="D62" s="2">
+      <c r="C62" s="5"/>
+      <c r="D62" s="1">
         <v>21.0</v>
       </c>
-      <c r="E62" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="F62" s="2">
+      <c r="E62" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="K62" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L62" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M62" s="2">
         <v>36.0</v>
       </c>
-      <c r="G62" s="5">
+      <c r="N62" s="6">
         <v>32177.0</v>
       </c>
-      <c r="I62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M62" s="2">
+      <c r="P62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T62" s="2">
         <v>29.0</v>
       </c>
-      <c r="N62" s="5">
+      <c r="U62" s="6">
         <v>43155.0</v>
       </c>
-      <c r="O62" s="2" t="s">
+      <c r="V62" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P62" s="5"/>
+      <c r="W62" s="6"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
@@ -2979,25 +3420,30 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="C63" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F63" s="2">
+      <c r="C63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M63" s="2">
         <v>48.0</v>
       </c>
-      <c r="G63" s="5">
+      <c r="N63" s="6">
         <v>656232.0</v>
       </c>
-      <c r="I63" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M63" s="2">
+      <c r="P63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T63" s="2">
         <v>44.0</v>
       </c>
-      <c r="N63" s="5">
+      <c r="U63" s="6">
         <v>341128.0</v>
       </c>
-      <c r="P63" s="5"/>
+      <c r="W63" s="6"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
@@ -3007,25 +3453,30 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="C64" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F64" s="2">
+      <c r="C64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M64" s="2">
         <v>45.0</v>
       </c>
-      <c r="G64" s="5">
+      <c r="N64" s="6">
         <v>29361.0</v>
       </c>
-      <c r="I64" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M64" s="2">
+      <c r="P64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T64" s="2">
         <v>38.0</v>
       </c>
-      <c r="N64" s="5">
+      <c r="U64" s="6">
         <v>14120.0</v>
       </c>
-      <c r="P64" s="5"/>
+      <c r="W64" s="6"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
@@ -3035,25 +3486,30 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="C65" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F65" s="2">
+      <c r="C65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M65" s="2">
         <v>41.0</v>
       </c>
-      <c r="G65" s="5">
+      <c r="N65" s="6">
         <v>113457.0</v>
       </c>
-      <c r="I65" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M65" s="2">
+      <c r="P65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T65" s="2">
         <v>40.0</v>
       </c>
-      <c r="N65" s="5">
+      <c r="U65" s="6">
         <v>73857.0</v>
       </c>
-      <c r="P65" s="5"/>
+      <c r="W65" s="6"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
@@ -3063,25 +3519,30 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="C66" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F66" s="2">
+      <c r="C66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M66" s="2">
         <v>45.0</v>
       </c>
-      <c r="G66" s="5">
+      <c r="N66" s="6">
         <v>454665.0</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M66" s="2">
+      <c r="P66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T66" s="2">
         <v>38.0</v>
       </c>
-      <c r="N66" s="5">
+      <c r="U66" s="6">
         <v>267534.0</v>
       </c>
-      <c r="P66" s="5"/>
+      <c r="W66" s="6"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
@@ -3091,28 +3552,33 @@
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="C67" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F67" s="2">
+      <c r="C67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M67" s="2">
         <v>47.0</v>
       </c>
-      <c r="G67" s="5">
+      <c r="N67" s="6">
         <v>130274.0</v>
       </c>
-      <c r="I67" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M67" s="2">
+      <c r="P67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T67" s="2">
         <v>45.0</v>
       </c>
-      <c r="N67" s="5">
+      <c r="U67" s="6">
         <v>76907.0</v>
       </c>
-      <c r="O67" s="2" t="s">
+      <c r="V67" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="P67" s="5"/>
+      <c r="W67" s="6"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
@@ -3122,25 +3588,30 @@
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="C68" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F68" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="G68" s="5">
+      <c r="C68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M68" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="N68" s="6">
         <v>402440.0</v>
       </c>
-      <c r="I68" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M68" s="2">
+      <c r="P68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T68" s="2">
         <v>45.0</v>
       </c>
-      <c r="N68" s="5">
+      <c r="U68" s="6">
         <v>184961.0</v>
       </c>
-      <c r="P68" s="5"/>
+      <c r="W68" s="6"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
@@ -3150,28 +3621,33 @@
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="C69" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="F69" s="2">
+      <c r="C69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="M69" s="2">
         <v>40.0</v>
       </c>
-      <c r="G69" s="5">
+      <c r="N69" s="6">
         <v>228145.0</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M69" s="2">
+      <c r="P69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T69" s="2">
         <v>41.0</v>
       </c>
-      <c r="N69" s="5">
+      <c r="U69" s="6">
         <v>138303.0</v>
       </c>
-      <c r="O69" s="2" t="s">
+      <c r="V69" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="P69" s="5"/>
+      <c r="W69" s="6"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
@@ -3181,15 +3657,20 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="C70" s="4">
-        <v>44308.0</v>
-      </c>
+      <c r="C70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-      <c r="M70" s="8">
-        <f t="shared" ref="M70:N70" si="2">average(M2:M69)</f>
+      <c r="J70" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="P70" s="6"/>
+      <c r="T70" s="9">
+        <f t="shared" ref="T70:U70" si="2">average(T2:T69)</f>
         <v>36.23076923</v>
       </c>
-      <c r="N70" s="8">
+      <c r="U70" s="9">
         <f t="shared" si="2"/>
         <v>79060.23077</v>
       </c>
@@ -3202,11 +3683,16 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="C71" s="4">
-        <v>44308.0</v>
-      </c>
-      <c r="M71" s="8">
-        <f>countif(M2:M69,"&gt;30")</f>
+      <c r="C71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5">
+        <v>44308.0</v>
+      </c>
+      <c r="T71" s="9">
+        <f>countif(T2:T69,"&gt;30")</f>
         <v>50</v>
       </c>
     </row>
@@ -3218,7 +3704,12 @@
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5">
         <v>44308.0</v>
       </c>
     </row>
@@ -3230,7 +3721,12 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5">
         <v>44308.0</v>
       </c>
     </row>
@@ -3242,7 +3738,12 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5">
         <v>44308.0</v>
       </c>
     </row>
@@ -3254,7 +3755,12 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5">
         <v>44308.0</v>
       </c>
     </row>
@@ -3266,7 +3772,12 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5">
         <v>44308.0</v>
       </c>
     </row>
@@ -3302,16 +3813,22 @@
       <c r="E79" s="2">
         <v>50.0</v>
       </c>
-      <c r="F79" s="2">
+      <c r="K79" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L79" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M79" s="2">
         <v>24.0</v>
       </c>
-      <c r="G79" s="5">
+      <c r="N79" s="6">
         <v>154752.0</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="O79" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I79" s="9">
+      <c r="P79" s="10">
         <v>12253.0</v>
       </c>
     </row>
@@ -3341,10 +3858,10 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="G82" s="9">
+      <c r="N82" s="10">
         <v>88458.0</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="P82" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3392,10 +3909,10 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="G87" s="9">
+      <c r="N87" s="10">
         <v>444821.0</v>
       </c>
-      <c r="I87" s="5" t="s">
+      <c r="P87" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3407,10 +3924,10 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="G88" s="9">
+      <c r="N88" s="10">
         <v>44297.0</v>
       </c>
-      <c r="I88" s="5" t="s">
+      <c r="P88" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3440,16 +3957,16 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="F91" s="2">
+      <c r="M91" s="2">
         <v>15.0</v>
       </c>
-      <c r="G91" s="5">
+      <c r="N91" s="6">
         <v>13659.0</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="O91" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I91" s="5" t="s">
+      <c r="P91" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3461,16 +3978,16 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="F92" s="2">
+      <c r="M92" s="2">
         <v>23.0</v>
       </c>
-      <c r="G92" s="5">
+      <c r="N92" s="6">
         <v>303318.0</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="O92" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I92" s="5" t="s">
+      <c r="P92" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3482,13 +3999,13 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="F93" s="2">
+      <c r="M93" s="2">
         <v>45.0</v>
       </c>
-      <c r="G93" s="5">
+      <c r="N93" s="6">
         <v>131817.0</v>
       </c>
-      <c r="I93" s="5" t="s">
+      <c r="P93" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3509,13 +4026,13 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="F95" s="2">
+      <c r="M95" s="2">
         <v>40.0</v>
       </c>
-      <c r="G95" s="5">
+      <c r="N95" s="6">
         <v>143248.0</v>
       </c>
-      <c r="I95" s="9" t="s">
+      <c r="P95" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3545,13 +4062,13 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="F98" s="2">
+      <c r="M98" s="2">
         <v>44.0</v>
       </c>
-      <c r="G98" s="9">
+      <c r="N98" s="10">
         <v>361004.0</v>
       </c>
-      <c r="I98" s="9" t="s">
+      <c r="P98" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3607,16 +4124,16 @@
       <c r="B104" s="2">
         <v>103.0</v>
       </c>
-      <c r="F104" s="2">
+      <c r="M104" s="2">
         <v>43.0</v>
       </c>
-      <c r="G104" s="5">
+      <c r="N104" s="6">
         <v>198773.0</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="O104" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I104" s="5" t="s">
+      <c r="P104" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3627,16 +4144,16 @@
       <c r="B105" s="2">
         <v>104.0</v>
       </c>
-      <c r="F105" s="2">
+      <c r="M105" s="2">
         <v>13.0</v>
       </c>
-      <c r="G105" s="5">
+      <c r="N105" s="6">
         <v>26879.0</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="O105" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I105" s="5" t="s">
+      <c r="P105" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3647,16 +4164,16 @@
       <c r="B106" s="2">
         <v>105.0</v>
       </c>
-      <c r="F106" s="2">
+      <c r="M106" s="2">
         <v>45.0</v>
       </c>
-      <c r="G106" s="5">
+      <c r="N106" s="6">
         <v>93917.0</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="O106" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I106" s="5" t="s">
+      <c r="P106" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3667,16 +4184,16 @@
       <c r="B107" s="2">
         <v>106.0</v>
       </c>
-      <c r="F107" s="2">
+      <c r="M107" s="2">
         <v>48.0</v>
       </c>
-      <c r="G107" s="5">
+      <c r="N107" s="6">
         <v>116076.0</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="O107" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I107" s="9" t="s">
+      <c r="P107" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3687,16 +4204,16 @@
       <c r="B108" s="2">
         <v>107.0</v>
       </c>
-      <c r="F108" s="2">
+      <c r="M108" s="2">
         <v>47.0</v>
       </c>
-      <c r="G108" s="5">
+      <c r="N108" s="6">
         <v>189271.0</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="O108" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I108" s="9" t="s">
+      <c r="P108" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3707,16 +4224,16 @@
       <c r="B109" s="2">
         <v>108.0</v>
       </c>
-      <c r="F109" s="2">
+      <c r="M109" s="2">
         <v>22.0</v>
       </c>
-      <c r="G109" s="5">
+      <c r="N109" s="6">
         <v>11157.0</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="O109" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I109" s="9" t="s">
+      <c r="P109" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3727,13 +4244,13 @@
       <c r="B110" s="2">
         <v>109.0</v>
       </c>
-      <c r="F110" s="2">
+      <c r="M110" s="2">
         <v>41.0</v>
       </c>
-      <c r="G110" s="5">
+      <c r="N110" s="6">
         <v>128775.0</v>
       </c>
-      <c r="I110" s="9" t="s">
+      <c r="P110" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3744,13 +4261,13 @@
       <c r="B111" s="2">
         <v>110.0</v>
       </c>
-      <c r="F111" s="2">
+      <c r="M111" s="2">
         <v>35.0</v>
       </c>
-      <c r="G111" s="5">
+      <c r="N111" s="6">
         <v>433534.0</v>
       </c>
-      <c r="I111" s="9" t="s">
+      <c r="P111" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3761,16 +4278,16 @@
       <c r="B112" s="2">
         <v>111.0</v>
       </c>
-      <c r="F112" s="2">
+      <c r="M112" s="2">
         <v>43.0</v>
       </c>
-      <c r="G112" s="5">
+      <c r="N112" s="6">
         <v>49224.0</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="O112" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I112" s="9" t="s">
+      <c r="P112" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3787,16 +4304,22 @@
       <c r="E113" s="2">
         <v>50.0</v>
       </c>
-      <c r="F113" s="2">
+      <c r="K113" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="L113" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="M113" s="2">
         <v>11.0</v>
       </c>
-      <c r="G113" s="5">
+      <c r="N113" s="6">
         <v>80467.0</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="O113" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="I113" s="9">
+      <c r="P113" s="10">
         <v>23938.0</v>
       </c>
     </row>
@@ -3825,12 +4348,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1000 M1:M1000">
+  <conditionalFormatting sqref="F1 M1:M1000 T1:T1000">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1000 M1:M20 P21 M22:M1000">
+  <conditionalFormatting sqref="F1 M1:M1000 T1:T20 W21 T22:T1000">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated params for 157
</commit_message>
<xml_diff>
--- a/data/detector_parameters.xlsx
+++ b/data/detector_parameters.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinconrad/Desktop/research/interictal_hubs/scripts/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70F962C-A21C-984E-8701-EFD429EBA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2380" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -493,32 +502,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -526,7 +540,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -536,78 +550,65 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -797,28 +798,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="22" max="22" width="14.86"/>
+    <col min="22" max="22" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,15 +893,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4">
-        <v>44316.0</v>
+        <v>44316</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -906,45 +910,45 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="N2" s="6">
-        <v>4078.0</v>
+        <v>4078</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q2" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R2" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S2" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T2" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="U2" s="6">
-        <v>2760.0</v>
+        <v>2760</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
@@ -954,42 +958,42 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N3" s="6">
-        <v>4783.0</v>
+        <v>4783</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q3" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R3" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S3" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T3" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="U3" s="2">
-        <v>2846.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
@@ -999,15 +1003,15 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="N4" s="6">
-        <v>1175.0</v>
+        <v>1175</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>14</v>
@@ -1016,30 +1020,30 @@
         <v>10</v>
       </c>
       <c r="Q4" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R4" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S4" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T4" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="U4" s="2">
-        <v>4501.0</v>
+        <v>4501</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
@@ -1049,43 +1053,43 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N5" s="6">
-        <v>146527.0</v>
+        <v>146527</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q5" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R5" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S5" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T5" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="U5" s="6">
-        <v>69816.0</v>
+        <v>69816</v>
       </c>
       <c r="V5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5"/>
@@ -1093,59 +1097,59 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M6" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="N6" s="6">
-        <v>50562.0</v>
+        <v>50562</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T6" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="U6" s="6">
-        <v>29593.0</v>
+        <v>29593</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K7" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L7" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M7" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N7" s="6">
-        <v>9967.0</v>
+        <v>9967</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>20</v>
@@ -1154,30 +1158,30 @@
         <v>10</v>
       </c>
       <c r="Q7" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R7" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="S7" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T7" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="U7" s="6">
-        <v>13737.0</v>
+        <v>13737</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
@@ -1187,121 +1191,121 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="N8" s="6">
-        <v>72449.0</v>
+        <v>72449</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q8" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R8" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S8" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T8" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="U8" s="6">
-        <v>34834.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>34834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K9" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L9" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M9" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="N9" s="6">
-        <v>74165.0</v>
+        <v>74165</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q9" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R9" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="S9" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T9" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="U9" s="6">
-        <v>42244.0</v>
+        <v>42244</v>
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K10" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L10" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M10" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="N10" s="6">
-        <v>139153.0</v>
+        <v>139153</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>24</v>
@@ -1310,31 +1314,31 @@
         <v>10</v>
       </c>
       <c r="Q10" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R10" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S10" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T10" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="U10" s="6">
-        <v>121330.0</v>
+        <v>121330</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="W10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ref="B11:B103" si="1">B10+1</f>
+        <f t="shared" ref="B11:B103" si="0">B10+1</f>
         <v>10</v>
       </c>
       <c r="C11" s="5"/>
@@ -1345,43 +1349,43 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="N11" s="6">
-        <v>47905.0</v>
+        <v>47905</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q11" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R11" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S11" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T11" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="U11" s="6">
-        <v>24791.0</v>
+        <v>24791</v>
       </c>
       <c r="W11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C12" s="5"/>
@@ -1392,15 +1396,15 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="N12" s="6">
-        <v>45278.0</v>
+        <v>45278</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>28</v>
@@ -1410,22 +1414,22 @@
       </c>
       <c r="Q12" s="5"/>
       <c r="T12" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="U12" s="6">
-        <v>22628.0</v>
+        <v>22628</v>
       </c>
       <c r="V12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="W12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
@@ -1436,15 +1440,15 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N13" s="6">
-        <v>89380.0</v>
+        <v>89380</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>31</v>
@@ -1453,31 +1457,31 @@
         <v>10</v>
       </c>
       <c r="Q13" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R13" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S13" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T13" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U13" s="6">
-        <v>44032.0</v>
+        <v>44032</v>
       </c>
       <c r="V13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W13" s="6"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
@@ -1488,15 +1492,15 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="N14" s="6">
-        <v>184199.0</v>
+        <v>184199</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>34</v>
@@ -1505,31 +1509,31 @@
         <v>10</v>
       </c>
       <c r="Q14" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R14" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S14" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T14" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="U14" s="6">
-        <v>89583.0</v>
+        <v>89583</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C15" s="5"/>
@@ -1538,13 +1542,13 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M15" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N15" s="6">
-        <v>9446.0</v>
+        <v>9446</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>36</v>
@@ -1553,74 +1557,74 @@
         <v>10</v>
       </c>
       <c r="T15" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U15" s="6">
-        <v>3006.0</v>
+        <v>3006</v>
       </c>
       <c r="W15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L16" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M16" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="N16" s="6">
-        <v>91233.0</v>
+        <v>91233</v>
       </c>
       <c r="O16" s="5"/>
       <c r="P16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q16" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="S16" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T16" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U16" s="6">
-        <v>47298.0</v>
+        <v>47298</v>
       </c>
       <c r="W16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C17" s="5"/>
@@ -1631,97 +1635,97 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="N17" s="6">
-        <v>34198.0</v>
+        <v>34198</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q17" s="5">
-        <v>44300.0</v>
+        <v>44300</v>
       </c>
       <c r="R17" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S17" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T17" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="U17" s="6">
-        <v>17693.0</v>
+        <v>17693</v>
       </c>
       <c r="W17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K18" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="L18" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M18" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="N18" s="6">
-        <v>198745.0</v>
+        <v>198745</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q18" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R18" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="S18" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T18" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="U18" s="6">
-        <v>29807.0</v>
+        <v>29807</v>
       </c>
       <c r="W18" s="6"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C19" s="5"/>
@@ -1730,31 +1734,31 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M19" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="N19" s="6">
-        <v>87137.0</v>
+        <v>87137</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T19" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="U19" s="6">
-        <v>44654.0</v>
+        <v>44654</v>
       </c>
       <c r="W19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C20" s="5"/>
@@ -1765,43 +1769,43 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="N20" s="6">
-        <v>90746.0</v>
+        <v>90746</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q20" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R20" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S20" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T20" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="U20" s="6">
-        <v>43574.0</v>
+        <v>43574</v>
       </c>
       <c r="W20" s="6"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C21" s="5"/>
@@ -1812,43 +1816,43 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="N21" s="6">
-        <v>371968.0</v>
+        <v>371968</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q21" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R21" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S21" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T21" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="U21" s="6">
-        <v>208828.0</v>
+        <v>208828</v>
       </c>
       <c r="W21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C22" s="5"/>
@@ -1859,43 +1863,43 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="N22" s="6">
-        <v>49715.0</v>
+        <v>49715</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q22" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R22" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S22" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T22" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U22" s="6">
-        <v>25937.0</v>
+        <v>25937</v>
       </c>
       <c r="W22" s="6"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C23" s="5"/>
@@ -1906,43 +1910,43 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="N23" s="6">
-        <v>94881.0</v>
+        <v>94881</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q23" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R23" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S23" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T23" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U23" s="6">
-        <v>47765.0</v>
+        <v>47765</v>
       </c>
       <c r="W23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C24" s="5"/>
@@ -1953,43 +1957,43 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="N24" s="6">
-        <v>114142.0</v>
+        <v>114142</v>
       </c>
       <c r="O24" s="5"/>
       <c r="P24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q24" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R24" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S24" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T24" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="U24" s="6">
-        <v>69257.0</v>
+        <v>69257</v>
       </c>
       <c r="W24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C25" s="5"/>
@@ -1998,7 +2002,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>47</v>
@@ -2007,12 +2011,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C26" s="5"/>
@@ -2021,7 +2025,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>47</v>
@@ -2030,12 +2034,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C27" s="5"/>
@@ -2044,31 +2048,31 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M27" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N27" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T27" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U27" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="W27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C28" s="5"/>
@@ -2077,31 +2081,31 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M28" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="N28" s="6">
-        <v>92315.0</v>
+        <v>92315</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T28" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="U28" s="6">
-        <v>50898.0</v>
+        <v>50898</v>
       </c>
       <c r="W28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C29" s="5"/>
@@ -2112,43 +2116,43 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="N29" s="6">
-        <v>29731.0</v>
+        <v>29731</v>
       </c>
       <c r="O29" s="5"/>
       <c r="P29" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Q29" s="5">
-        <v>44301.0</v>
+        <v>44301</v>
       </c>
       <c r="R29" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="S29" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="T29" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="U29" s="6">
-        <v>16039.0</v>
+        <v>16039</v>
       </c>
       <c r="W29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C30" s="5"/>
@@ -2157,13 +2161,13 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M30" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N30" s="6">
-        <v>68836.0</v>
+        <v>68836</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>54</v>
@@ -2172,19 +2176,19 @@
         <v>10</v>
       </c>
       <c r="T30" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="U30" s="6">
-        <v>32888.0</v>
+        <v>32888</v>
       </c>
       <c r="W30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C31" s="5"/>
@@ -2193,31 +2197,31 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M31" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N31" s="6">
-        <v>929822.0</v>
+        <v>929822</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T31" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="U31" s="6">
-        <v>473121.0</v>
+        <v>473121</v>
       </c>
       <c r="W31" s="6"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C32" s="5"/>
@@ -2226,34 +2230,34 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M32" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N32" s="6">
-        <v>97622.0</v>
+        <v>97622</v>
       </c>
       <c r="P32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T32" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="U32" s="6">
-        <v>51057.0</v>
+        <v>51057</v>
       </c>
       <c r="V32" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C33" s="5"/>
@@ -2262,7 +2266,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>47</v>
@@ -2272,12 +2276,12 @@
       </c>
       <c r="W33" s="6"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="C34" s="5"/>
@@ -2286,31 +2290,31 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M34" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="N34" s="6">
-        <v>286766.0</v>
+        <v>286766</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T34" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="U34" s="6">
-        <v>145929.0</v>
+        <v>145929</v>
       </c>
       <c r="W34" s="6"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="C35" s="5"/>
@@ -2319,31 +2323,31 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M35" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="N35" s="6">
-        <v>139716.0</v>
+        <v>139716</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T35" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="U35" s="6">
-        <v>73965.0</v>
+        <v>73965</v>
       </c>
       <c r="W35" s="6"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C36" s="5"/>
@@ -2352,13 +2356,13 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M36" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="N36" s="6">
-        <v>191825.0</v>
+        <v>191825</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>54</v>
@@ -2367,22 +2371,22 @@
         <v>10</v>
       </c>
       <c r="T36" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="U36" s="6">
-        <v>98347.0</v>
+        <v>98347</v>
       </c>
       <c r="V36" s="2" t="s">
         <v>62</v>
       </c>
       <c r="W36" s="6"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C37" s="5"/>
@@ -2391,13 +2395,13 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M37" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="N37" s="6">
-        <v>28580.0</v>
+        <v>28580</v>
       </c>
       <c r="O37" s="2" t="s">
         <v>64</v>
@@ -2406,49 +2410,49 @@
         <v>10</v>
       </c>
       <c r="T37" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="U37" s="6">
-        <v>14088.0</v>
+        <v>14088</v>
       </c>
       <c r="V37" s="2" t="s">
         <v>65</v>
       </c>
       <c r="W37" s="6"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K38" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L38" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M38" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="N38" s="6">
-        <v>6532.0</v>
+        <v>6532</v>
       </c>
       <c r="O38" s="2" t="s">
         <v>64</v>
@@ -2457,70 +2461,70 @@
         <v>10</v>
       </c>
       <c r="T38" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="U38" s="6">
-        <v>10262.0</v>
+        <v>10262</v>
       </c>
       <c r="V38" s="2" t="s">
         <v>65</v>
       </c>
       <c r="W38" s="6"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E39" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K39" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L39" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M39" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N39" s="6">
-        <v>23033.0</v>
+        <v>23033</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T39" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="U39" s="6">
-        <v>30333.0</v>
+        <v>30333</v>
       </c>
       <c r="V39" s="2" t="s">
         <v>65</v>
       </c>
       <c r="W39" s="6"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="C40" s="5"/>
@@ -2529,34 +2533,34 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M40" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="N40" s="6">
-        <v>34375.0</v>
+        <v>34375</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T40" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="U40" s="6">
-        <v>20684.0</v>
+        <v>20684</v>
       </c>
       <c r="V40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W40" s="6"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C41" s="5"/>
@@ -2565,13 +2569,13 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M41" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="N41" s="6">
-        <v>150601.0</v>
+        <v>150601</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>54</v>
@@ -2580,22 +2584,22 @@
         <v>10</v>
       </c>
       <c r="T41" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="U41" s="6">
-        <v>79119.0</v>
+        <v>79119</v>
       </c>
       <c r="V41" s="2" t="s">
         <v>57</v>
       </c>
       <c r="W41" s="6"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="C42" s="5"/>
@@ -2604,13 +2608,13 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M42" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="N42" s="6">
-        <v>26145.0</v>
+        <v>26145</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>54</v>
@@ -2619,22 +2623,22 @@
         <v>10</v>
       </c>
       <c r="T42" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="U42" s="6">
-        <v>10456.0</v>
+        <v>10456</v>
       </c>
       <c r="V42" s="2" t="s">
         <v>71</v>
       </c>
       <c r="W42" s="6"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C43" s="5"/>
@@ -2643,34 +2647,34 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M43" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="N43" s="6">
-        <v>136012.0</v>
+        <v>136012</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T43" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="U43" s="6">
-        <v>78393.0</v>
+        <v>78393</v>
       </c>
       <c r="V43" s="2" t="s">
         <v>62</v>
       </c>
       <c r="W43" s="6"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="C44" s="5"/>
@@ -2679,34 +2683,34 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M44" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N44" s="6">
-        <v>224824.0</v>
+        <v>224824</v>
       </c>
       <c r="P44" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T44" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="U44" s="6">
-        <v>123171.0</v>
+        <v>123171</v>
       </c>
       <c r="V44" s="2" t="s">
         <v>62</v>
       </c>
       <c r="W44" s="6"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="C45" s="5"/>
@@ -2715,13 +2719,13 @@
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M45" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="N45" s="6">
-        <v>37736.0</v>
+        <v>37736</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>54</v>
@@ -2730,67 +2734,67 @@
         <v>10</v>
       </c>
       <c r="T45" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="U45" s="6">
-        <v>16938.0</v>
+        <v>16938</v>
       </c>
       <c r="W45" s="6"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E46" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K46" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L46" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M46" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="N46" s="6">
-        <v>9527.0</v>
+        <v>9527</v>
       </c>
       <c r="P46" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T46" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="U46" s="6">
-        <v>14524.0</v>
+        <v>14524</v>
       </c>
       <c r="V46" s="2" t="s">
         <v>65</v>
       </c>
       <c r="W46" s="6"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="C47" s="5"/>
@@ -2799,13 +2803,13 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M47" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="N47" s="6">
-        <v>121224.0</v>
+        <v>121224</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>54</v>
@@ -2814,22 +2818,22 @@
         <v>10</v>
       </c>
       <c r="T47" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="U47" s="6">
-        <v>61054.0</v>
+        <v>61054</v>
       </c>
       <c r="V47" s="2" t="s">
         <v>62</v>
       </c>
       <c r="W47" s="6"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="C48" s="5"/>
@@ -2838,13 +2842,13 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M48" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N48" s="6">
-        <v>32458.0</v>
+        <v>32458</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>54</v>
@@ -2853,22 +2857,22 @@
         <v>10</v>
       </c>
       <c r="T48" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="U48" s="6">
-        <v>15524.0</v>
+        <v>15524</v>
       </c>
       <c r="V48" s="2" t="s">
         <v>78</v>
       </c>
       <c r="W48" s="6"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C49" s="5"/>
@@ -2877,13 +2881,13 @@
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M49" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N49" s="6">
-        <v>156752.0</v>
+        <v>156752</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>54</v>
@@ -2892,55 +2896,61 @@
         <v>10</v>
       </c>
       <c r="T49" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="U49" s="6">
-        <v>83327.0</v>
+        <v>83327</v>
       </c>
       <c r="W49" s="6"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C50" s="5"/>
+      <c r="D50">
+        <v>21</v>
+      </c>
+      <c r="E50">
+        <v>50</v>
+      </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M50" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N50" s="6">
-        <v>642448.0</v>
+        <v>642448</v>
       </c>
       <c r="P50" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T50" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="U50" s="6">
-        <v>342798.0</v>
+        <v>342798</v>
       </c>
       <c r="V50" s="2" t="s">
         <v>81</v>
       </c>
       <c r="W50" s="6"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="C51" s="5"/>
@@ -2949,154 +2959,154 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M51" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="N51" s="6">
-        <v>240248.0</v>
+        <v>240248</v>
       </c>
       <c r="P51" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T51" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="U51" s="6">
-        <v>123368.0</v>
+        <v>123368</v>
       </c>
       <c r="W51" s="6"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E52" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K52" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L52" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M52" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="N52" s="6">
-        <v>22740.0</v>
+        <v>22740</v>
       </c>
       <c r="P52" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T52" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="U52" s="6">
-        <v>36215.0</v>
+        <v>36215</v>
       </c>
       <c r="V52" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W52" s="6"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E53" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K53" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L53" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M53" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="N53" s="6">
-        <v>125235.0</v>
+        <v>125235</v>
       </c>
       <c r="P53" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T53" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="U53" s="6">
-        <v>144883.0</v>
+        <v>144883</v>
       </c>
       <c r="V53" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W53" s="6"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E54" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K54" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L54" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M54" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="N54" s="6">
-        <v>59220.0</v>
+        <v>59220</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>87</v>
@@ -3105,22 +3115,22 @@
         <v>10</v>
       </c>
       <c r="T54" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="U54" s="6">
-        <v>68393.0</v>
+        <v>68393</v>
       </c>
       <c r="V54" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W54" s="6"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C55" s="5"/>
@@ -3129,31 +3139,31 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M55" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="N55" s="6">
-        <v>335747.0</v>
+        <v>335747</v>
       </c>
       <c r="P55" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T55" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="U55" s="6">
-        <v>214741.0</v>
+        <v>214741</v>
       </c>
       <c r="W55" s="6"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C56" s="5"/>
@@ -3162,34 +3172,34 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M56" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="N56" s="6">
-        <v>147845.0</v>
+        <v>147845</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T56" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="U56" s="2">
-        <v>87323.0</v>
+        <v>87323</v>
       </c>
       <c r="V56" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W56" s="6"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B57" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C57" s="5"/>
@@ -3198,31 +3208,31 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M57" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="N57" s="6">
-        <v>70184.0</v>
+        <v>70184</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T57" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="U57" s="6">
-        <v>41956.0</v>
+        <v>41956</v>
       </c>
       <c r="W57" s="6"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B58" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C58" s="5"/>
@@ -3231,31 +3241,31 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M58" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N58" s="6">
-        <v>380459.0</v>
+        <v>380459</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T58" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="U58" s="6">
-        <v>236914.0</v>
+        <v>236914</v>
       </c>
       <c r="W58" s="6"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B59" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C59" s="5"/>
@@ -3264,79 +3274,79 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M59" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="N59" s="6">
-        <v>143117.0</v>
+        <v>143117</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T59" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="U59" s="6">
-        <v>83045.0</v>
+        <v>83045</v>
       </c>
       <c r="W59" s="6"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B60" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E60" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K60" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L60" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M60" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="N60" s="6">
-        <v>3108.0</v>
+        <v>3108</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T60" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="U60" s="6">
-        <v>6985.0</v>
+        <v>6985</v>
       </c>
       <c r="V60" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W60" s="6"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B61" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="C61" s="5"/>
@@ -3345,79 +3355,79 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M61" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="N61" s="6">
-        <v>120105.0</v>
+        <v>120105</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T61" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="U61" s="6">
-        <v>71698.0</v>
+        <v>71698</v>
       </c>
       <c r="W61" s="6"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B62" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E62" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="K62" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L62" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M62" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="N62" s="6">
-        <v>32177.0</v>
+        <v>32177</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T62" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="U62" s="6">
-        <v>43155.0</v>
+        <v>43155</v>
       </c>
       <c r="V62" s="2" t="s">
         <v>84</v>
       </c>
       <c r="W62" s="6"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B63" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="C63" s="5"/>
@@ -3426,31 +3436,31 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M63" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N63" s="6">
-        <v>656232.0</v>
+        <v>656232</v>
       </c>
       <c r="P63" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T63" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="U63" s="6">
-        <v>341128.0</v>
+        <v>341128</v>
       </c>
       <c r="W63" s="6"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B64" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="C64" s="5"/>
@@ -3459,31 +3469,31 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M64" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N64" s="6">
-        <v>29361.0</v>
+        <v>29361</v>
       </c>
       <c r="P64" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T64" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="U64" s="6">
-        <v>14120.0</v>
+        <v>14120</v>
       </c>
       <c r="W64" s="6"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B65" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="C65" s="5"/>
@@ -3492,31 +3502,31 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M65" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="N65" s="6">
-        <v>113457.0</v>
+        <v>113457</v>
       </c>
       <c r="P65" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T65" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="U65" s="6">
-        <v>73857.0</v>
+        <v>73857</v>
       </c>
       <c r="W65" s="6"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B66" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="C66" s="5"/>
@@ -3525,31 +3535,31 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M66" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N66" s="6">
-        <v>454665.0</v>
+        <v>454665</v>
       </c>
       <c r="P66" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T66" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="U66" s="6">
-        <v>267534.0</v>
+        <v>267534</v>
       </c>
       <c r="W66" s="6"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B67" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="C67" s="5"/>
@@ -3558,34 +3568,34 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M67" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="N67" s="6">
-        <v>130274.0</v>
+        <v>130274</v>
       </c>
       <c r="P67" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T67" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="U67" s="6">
-        <v>76907.0</v>
+        <v>76907</v>
       </c>
       <c r="V67" s="2" t="s">
         <v>101</v>
       </c>
       <c r="W67" s="6"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B68" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="C68" s="5"/>
@@ -3594,31 +3604,31 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M68" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="N68" s="6">
-        <v>402440.0</v>
+        <v>402440</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T68" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="U68" s="6">
-        <v>184961.0</v>
+        <v>184961</v>
       </c>
       <c r="W68" s="6"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B69" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="C69" s="5"/>
@@ -3627,34 +3637,34 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="M69" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N69" s="6">
-        <v>228145.0</v>
+        <v>228145</v>
       </c>
       <c r="P69" s="6" t="s">
         <v>10</v>
       </c>
       <c r="T69" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="U69" s="6">
-        <v>138303.0</v>
+        <v>138303</v>
       </c>
       <c r="V69" s="2" t="s">
         <v>104</v>
       </c>
       <c r="W69" s="6"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="C70" s="5"/>
@@ -3663,24 +3673,24 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="P70" s="6"/>
       <c r="T70" s="9">
-        <f t="shared" ref="T70:U70" si="2">average(T2:T69)</f>
-        <v>36.23076923</v>
+        <f t="shared" ref="T70:U70" si="1">AVERAGE(T2:T69)</f>
+        <v>36.230769230769234</v>
       </c>
       <c r="U70" s="9">
-        <f t="shared" si="2"/>
-        <v>79060.23077</v>
-      </c>
-    </row>
-    <row r="71">
+        <f t="shared" si="1"/>
+        <v>79060.230769230766</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B71" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="C71" s="5"/>
@@ -3689,19 +3699,19 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5">
-        <v>44308.0</v>
+        <v>44308</v>
       </c>
       <c r="T71" s="9">
-        <f>countif(T2:T69,"&gt;30")</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72">
+        <f>COUNTIF(T2:T69,"&gt;30")</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B72" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="C72" s="5"/>
@@ -3710,15 +3720,15 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5">
-        <v>44308.0</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B73" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="C73" s="5"/>
@@ -3727,15 +3737,15 @@
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5">
-        <v>44308.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B74" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="C74" s="5"/>
@@ -3744,15 +3754,15 @@
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5">
-        <v>44308.0</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B75" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="C75" s="5"/>
@@ -3761,15 +3771,15 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5">
-        <v>44308.0</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B76" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="C76" s="5"/>
@@ -3778,190 +3788,190 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5">
-        <v>44308.0</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B77" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B78" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B79" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="D79" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E79" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K79" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L79" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M79" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="N79" s="6">
-        <v>154752.0</v>
+        <v>154752</v>
       </c>
       <c r="O79" s="2" t="s">
         <v>115</v>
       </c>
       <c r="P79" s="10">
-        <v>12253.0</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>12253</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B80" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B81" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B82" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="N82" s="10">
-        <v>88458.0</v>
+        <v>88458</v>
       </c>
       <c r="P82" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B83" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B84" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B85" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B86" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B87" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="N87" s="10">
-        <v>444821.0</v>
+        <v>444821</v>
       </c>
       <c r="P87" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B88" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="N88" s="10">
-        <v>44297.0</v>
+        <v>44297</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B89" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B90" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B91" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="M91" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="N91" s="6">
-        <v>13659.0</v>
+        <v>13659</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>128</v>
@@ -3970,19 +3980,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B92" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="M92" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="N92" s="6">
-        <v>303318.0</v>
+        <v>303318</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>130</v>
@@ -3991,144 +4001,144 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B93" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
       <c r="M93" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N93" s="6">
-        <v>131817.0</v>
+        <v>131817</v>
       </c>
       <c r="P93" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B94" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B95" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="M95" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="N95" s="6">
-        <v>143248.0</v>
+        <v>143248</v>
       </c>
       <c r="P95" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B96" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B97" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B98" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="M98" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="N98" s="10">
-        <v>361004.0</v>
+        <v>361004</v>
       </c>
       <c r="P98" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B99" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>98</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B100" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B101" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B102" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B103" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B104" s="2">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="M104" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="N104" s="6">
-        <v>198773.0</v>
+        <v>198773</v>
       </c>
       <c r="O104" s="2" t="s">
         <v>62</v>
@@ -4137,18 +4147,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B105" s="2">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="M105" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="N105" s="6">
-        <v>26879.0</v>
+        <v>26879</v>
       </c>
       <c r="O105" s="2" t="s">
         <v>144</v>
@@ -4157,18 +4167,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B106" s="2">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="M106" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="N106" s="6">
-        <v>93917.0</v>
+        <v>93917</v>
       </c>
       <c r="O106" s="2" t="s">
         <v>146</v>
@@ -4177,18 +4187,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B107" s="2">
-        <v>106.0</v>
+        <v>106</v>
       </c>
       <c r="M107" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="N107" s="6">
-        <v>116076.0</v>
+        <v>116076</v>
       </c>
       <c r="O107" s="2" t="s">
         <v>54</v>
@@ -4197,18 +4207,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B108" s="2">
-        <v>107.0</v>
+        <v>107</v>
       </c>
       <c r="M108" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="N108" s="6">
-        <v>189271.0</v>
+        <v>189271</v>
       </c>
       <c r="O108" s="2" t="s">
         <v>54</v>
@@ -4217,18 +4227,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B109" s="2">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="M109" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="N109" s="6">
-        <v>11157.0</v>
+        <v>11157</v>
       </c>
       <c r="O109" s="2" t="s">
         <v>150</v>
@@ -4237,52 +4247,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B110" s="2">
-        <v>109.0</v>
+        <v>109</v>
       </c>
       <c r="M110" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="N110" s="6">
-        <v>128775.0</v>
+        <v>128775</v>
       </c>
       <c r="P110" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B111" s="2">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="M111" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="N111" s="6">
-        <v>433534.0</v>
+        <v>433534</v>
       </c>
       <c r="P111" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B112" s="2">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="M112" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="N112" s="6">
-        <v>49224.0</v>
+        <v>49224</v>
       </c>
       <c r="O112" s="2" t="s">
         <v>54</v>
@@ -4291,73 +4301,73 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B113" s="2">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="D113" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E113" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K113" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="L113" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="M113" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="N113" s="6">
-        <v>80467.0</v>
+        <v>80467</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>155</v>
       </c>
       <c r="P113" s="10">
-        <v>23938.0</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>23938</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B114" s="2">
-        <v>113.0</v>
-      </c>
-    </row>
-    <row r="115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B115" s="2">
-        <v>114.0</v>
-      </c>
-    </row>
-    <row r="116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B116" s="2">
-        <v>115.0</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1 M1:M1000 T1:T1000">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1 M1:M1000 T1:T20 W21 T22:T1000">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>